<commit_message>
Data preparation and model calculation
</commit_message>
<xml_diff>
--- a/data/raw/data_raw.xlsx
+++ b/data/raw/data_raw.xlsx
@@ -1268,7 +1268,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1324,13 +1324,14 @@
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Komma 2" xfId="1"/>
@@ -1648,14 +1649,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AS126"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="P1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AK1" sqref="AK1:AK1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AL1" sqref="A1:AL101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="43" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" style="42" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="11.28515625" style="4" bestFit="1" customWidth="1"/>
@@ -1685,7 +1686,7 @@
     <col min="36" max="36" width="9.85546875" style="19" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="15" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="6" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="41" max="42" width="32.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="43" max="44" width="24.140625" style="2" bestFit="1" customWidth="1"/>
@@ -1827,7 +1828,7 @@
       </c>
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A2" s="42">
+      <c r="A2" s="41">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1927,17 +1928,21 @@
       <c r="AG2" s="40">
         <v>0.63670000000000004</v>
       </c>
-      <c r="AH2" s="44">
+      <c r="AH2" s="43">
         <v>107.2</v>
       </c>
-      <c r="AI2" s="44">
+      <c r="AI2" s="43">
         <v>82.5</v>
       </c>
-      <c r="AJ2" s="44">
+      <c r="AJ2" s="43">
         <v>112.5</v>
       </c>
-      <c r="AK2" s="33"/>
-      <c r="AL2" s="33"/>
+      <c r="AK2" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL2" s="45">
+        <v>134.4</v>
+      </c>
       <c r="AO2" s="2">
         <v>14.5</v>
       </c>
@@ -1952,7 +1957,7 @@
       </c>
     </row>
     <row r="3" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A3" s="42">
+      <c r="A3" s="41">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -2052,17 +2057,21 @@
       <c r="AG3" s="40">
         <v>0.25580000000000003</v>
       </c>
-      <c r="AH3" s="44">
+      <c r="AH3" s="43">
         <v>40.200000000000003</v>
       </c>
-      <c r="AI3" s="44">
+      <c r="AI3" s="43">
         <v>53.3</v>
       </c>
-      <c r="AJ3" s="44">
+      <c r="AJ3" s="43">
         <v>43.9</v>
       </c>
-      <c r="AK3" s="33"/>
-      <c r="AL3" s="33"/>
+      <c r="AK3" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL3" s="45">
+        <v>134.19999999999999</v>
+      </c>
       <c r="AO3" s="2">
         <v>18.8</v>
       </c>
@@ -2077,7 +2086,7 @@
       </c>
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A4" s="42">
+      <c r="A4" s="41">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -2177,17 +2186,21 @@
       <c r="AG4" s="40">
         <v>0.15090000000000001</v>
       </c>
-      <c r="AH4" s="44">
+      <c r="AH4" s="43">
         <v>34.392000000000003</v>
       </c>
-      <c r="AI4" s="44">
+      <c r="AI4" s="43">
         <v>32.317999999999998</v>
       </c>
-      <c r="AJ4" s="44">
+      <c r="AJ4" s="43">
         <v>29.013000000000002</v>
       </c>
-      <c r="AK4" s="33"/>
-      <c r="AL4" s="33"/>
+      <c r="AK4" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL4" s="45">
+        <v>96.6</v>
+      </c>
       <c r="AO4" s="2">
         <v>16.5</v>
       </c>
@@ -2202,7 +2215,7 @@
       </c>
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A5" s="42">
+      <c r="A5" s="41">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -2302,17 +2315,21 @@
       <c r="AG5" s="40">
         <v>9.1499999999999998E-2</v>
       </c>
-      <c r="AH5" s="44">
+      <c r="AH5" s="43">
         <v>24.4</v>
       </c>
-      <c r="AI5" s="44">
+      <c r="AI5" s="43">
         <v>22.3</v>
       </c>
-      <c r="AJ5" s="44">
+      <c r="AJ5" s="43">
         <v>22</v>
       </c>
-      <c r="AK5" s="33"/>
-      <c r="AL5" s="33"/>
+      <c r="AK5" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL5" s="45">
+        <v>102.8</v>
+      </c>
       <c r="AO5" s="2">
         <v>17.5</v>
       </c>
@@ -2327,7 +2344,7 @@
       </c>
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A6" s="42">
+      <c r="A6" s="41">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -2427,17 +2444,21 @@
       <c r="AG6" s="40">
         <v>0.60519999999999996</v>
       </c>
-      <c r="AH6" s="44">
+      <c r="AH6" s="43">
         <v>65.099999999999994</v>
       </c>
-      <c r="AI6" s="44">
+      <c r="AI6" s="43">
         <v>92.7</v>
       </c>
-      <c r="AJ6" s="44">
+      <c r="AJ6" s="43">
         <v>87.3</v>
       </c>
-      <c r="AK6" s="33"/>
-      <c r="AL6" s="33"/>
+      <c r="AK6" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL6" s="45">
+        <v>136.19999999999999</v>
+      </c>
       <c r="AO6" s="10">
         <v>12</v>
       </c>
@@ -2452,7 +2473,7 @@
       </c>
     </row>
     <row r="7" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A7" s="42">
+      <c r="A7" s="41">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -2552,17 +2573,21 @@
       <c r="AG7" s="40">
         <v>0.56740000000000002</v>
       </c>
-      <c r="AH7" s="44">
+      <c r="AH7" s="43">
         <v>102.2</v>
       </c>
-      <c r="AI7" s="44">
+      <c r="AI7" s="43">
         <v>73.400000000000006</v>
       </c>
-      <c r="AJ7" s="44">
+      <c r="AJ7" s="43">
         <v>83.6</v>
       </c>
-      <c r="AK7" s="33"/>
-      <c r="AL7" s="33"/>
+      <c r="AK7" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL7" s="45">
+        <v>158.80000000000001</v>
+      </c>
       <c r="AO7" s="8">
         <v>12.8</v>
       </c>
@@ -2577,7 +2602,7 @@
       </c>
     </row>
     <row r="8" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A8" s="42">
+      <c r="A8" s="41">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -2677,17 +2702,21 @@
       <c r="AG8" s="40">
         <v>9.6799999999999997E-2</v>
       </c>
-      <c r="AH8" s="44">
+      <c r="AH8" s="43">
         <v>33.4</v>
       </c>
-      <c r="AI8" s="44">
+      <c r="AI8" s="43">
         <v>31.1</v>
       </c>
-      <c r="AJ8" s="44">
+      <c r="AJ8" s="43">
         <v>17.100000000000001</v>
       </c>
-      <c r="AK8" s="33"/>
-      <c r="AL8" s="33"/>
+      <c r="AK8" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL8" s="45">
+        <v>190</v>
+      </c>
       <c r="AO8" s="8">
         <v>21.4</v>
       </c>
@@ -2702,7 +2731,7 @@
       </c>
     </row>
     <row r="9" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A9" s="42">
+      <c r="A9" s="41">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -2802,17 +2831,21 @@
       <c r="AG9" s="40">
         <v>0.13159999999999999</v>
       </c>
-      <c r="AH9" s="44">
+      <c r="AH9" s="43">
         <v>26.5</v>
       </c>
-      <c r="AI9" s="44">
+      <c r="AI9" s="43">
         <v>25.7</v>
       </c>
-      <c r="AJ9" s="44">
+      <c r="AJ9" s="43">
         <v>24.7</v>
       </c>
-      <c r="AK9" s="33"/>
-      <c r="AL9" s="33"/>
+      <c r="AK9" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL9" s="45">
+        <v>104.8</v>
+      </c>
       <c r="AO9" s="8">
         <v>15.8</v>
       </c>
@@ -2827,7 +2860,7 @@
       </c>
     </row>
     <row r="10" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A10" s="42">
+      <c r="A10" s="41">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -2927,17 +2960,21 @@
       <c r="AG10" s="40">
         <v>0.63529999999999998</v>
       </c>
-      <c r="AH10" s="44">
+      <c r="AH10" s="43">
         <v>85.3</v>
       </c>
-      <c r="AI10" s="44">
+      <c r="AI10" s="43">
         <v>47.2</v>
       </c>
-      <c r="AJ10" s="44">
+      <c r="AJ10" s="43">
         <v>92.3</v>
       </c>
-      <c r="AK10" s="33"/>
-      <c r="AL10" s="33"/>
+      <c r="AK10" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL10" s="45">
+        <v>112</v>
+      </c>
       <c r="AO10" s="8">
         <v>9.8000000000000007</v>
       </c>
@@ -2952,7 +2989,7 @@
       </c>
     </row>
     <row r="11" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A11" s="42">
+      <c r="A11" s="41">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -3052,17 +3089,21 @@
       <c r="AG11" s="40">
         <v>0.60660000000000003</v>
       </c>
-      <c r="AH11" s="44">
+      <c r="AH11" s="43">
         <v>217.9</v>
       </c>
-      <c r="AI11" s="44">
+      <c r="AI11" s="43">
         <v>160.4</v>
       </c>
-      <c r="AJ11" s="44">
+      <c r="AJ11" s="43">
         <v>85.9</v>
       </c>
-      <c r="AK11" s="33"/>
-      <c r="AL11" s="33"/>
+      <c r="AK11" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL11" s="45">
+        <v>167.2</v>
+      </c>
       <c r="AO11" s="8">
         <v>18.3</v>
       </c>
@@ -3077,7 +3118,7 @@
       </c>
     </row>
     <row r="12" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A12" s="42">
+      <c r="A12" s="41">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -3177,17 +3218,21 @@
       <c r="AG12" s="40">
         <v>0.15989999999999999</v>
       </c>
-      <c r="AH12" s="45">
+      <c r="AH12" s="44">
         <v>32.700000000000003</v>
       </c>
-      <c r="AI12" s="44">
+      <c r="AI12" s="43">
         <v>37.200000000000003</v>
       </c>
-      <c r="AJ12" s="44">
+      <c r="AJ12" s="43">
         <v>26.2</v>
       </c>
-      <c r="AK12" s="33"/>
-      <c r="AL12" s="33"/>
+      <c r="AK12" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL12" s="45">
+        <v>145.4</v>
+      </c>
       <c r="AO12" s="8">
         <v>16.7</v>
       </c>
@@ -3202,7 +3247,7 @@
       </c>
     </row>
     <row r="13" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A13" s="42">
+      <c r="A13" s="41">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -3302,17 +3347,21 @@
       <c r="AG13" s="40">
         <v>0.1726</v>
       </c>
-      <c r="AH13" s="44">
+      <c r="AH13" s="43">
         <v>47.3</v>
       </c>
-      <c r="AI13" s="44">
+      <c r="AI13" s="43">
         <v>46.6</v>
       </c>
-      <c r="AJ13" s="44">
+      <c r="AJ13" s="43">
         <v>31.4</v>
       </c>
-      <c r="AK13" s="33"/>
-      <c r="AL13" s="33"/>
+      <c r="AK13" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL13" s="45">
+        <v>185.4</v>
+      </c>
       <c r="AO13" s="8">
         <v>19.7</v>
       </c>
@@ -3327,7 +3376,7 @@
       </c>
     </row>
     <row r="14" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A14" s="42">
+      <c r="A14" s="41">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -3427,17 +3476,21 @@
       <c r="AG14" s="40">
         <v>0.62339999999999995</v>
       </c>
-      <c r="AH14" s="45">
+      <c r="AH14" s="44">
         <v>158.5</v>
       </c>
-      <c r="AI14" s="44">
+      <c r="AI14" s="43">
         <v>110.7</v>
       </c>
-      <c r="AJ14" s="44">
+      <c r="AJ14" s="43">
         <v>114.9</v>
       </c>
-      <c r="AK14" s="33"/>
-      <c r="AL14" s="33"/>
+      <c r="AK14" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL14" s="43">
+        <v>114.2</v>
+      </c>
       <c r="AO14" s="8">
         <v>9.6</v>
       </c>
@@ -3452,7 +3505,7 @@
       </c>
     </row>
     <row r="15" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A15" s="42">
+      <c r="A15" s="41">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -3552,17 +3605,21 @@
       <c r="AG15" s="40">
         <v>0.35949999999999999</v>
       </c>
-      <c r="AH15" s="44">
+      <c r="AH15" s="43">
         <v>103.2</v>
       </c>
-      <c r="AI15" s="44">
+      <c r="AI15" s="43">
         <v>80.7</v>
       </c>
-      <c r="AJ15" s="44">
+      <c r="AJ15" s="43">
         <v>72</v>
       </c>
-      <c r="AK15" s="33"/>
-      <c r="AL15" s="33"/>
+      <c r="AK15" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL15" s="45">
+        <v>163.6</v>
+      </c>
       <c r="AO15" s="8">
         <v>15.5</v>
       </c>
@@ -3577,7 +3634,7 @@
       </c>
     </row>
     <row r="16" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A16" s="42">
+      <c r="A16" s="41">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -3677,17 +3734,21 @@
       <c r="AG16" s="40">
         <v>0.1129</v>
       </c>
-      <c r="AH16" s="44">
+      <c r="AH16" s="43">
         <v>33.200000000000003</v>
       </c>
-      <c r="AI16" s="44">
+      <c r="AI16" s="43">
         <v>35.299999999999997</v>
       </c>
-      <c r="AJ16" s="44">
+      <c r="AJ16" s="43">
         <v>28.2</v>
       </c>
-      <c r="AK16" s="33"/>
-      <c r="AL16" s="33"/>
+      <c r="AK16" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL16" s="45">
+        <v>93</v>
+      </c>
       <c r="AO16" s="8">
         <v>15.2</v>
       </c>
@@ -3702,7 +3763,7 @@
       </c>
     </row>
     <row r="17" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A17" s="42">
+      <c r="A17" s="41">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -3802,17 +3863,21 @@
       <c r="AG17" s="40">
         <v>9.7500000000000003E-2</v>
       </c>
-      <c r="AH17" s="44">
+      <c r="AH17" s="43">
         <v>26.4</v>
       </c>
-      <c r="AI17" s="44">
+      <c r="AI17" s="43">
         <v>26.9</v>
       </c>
-      <c r="AJ17" s="44">
+      <c r="AJ17" s="43">
         <v>20.8</v>
       </c>
-      <c r="AK17" s="33"/>
-      <c r="AL17" s="33"/>
+      <c r="AK17" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL17" s="45">
+        <v>127.8</v>
+      </c>
       <c r="AO17" s="8">
         <v>21.4</v>
       </c>
@@ -3827,7 +3892,7 @@
       </c>
     </row>
     <row r="18" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A18" s="42">
+      <c r="A18" s="41">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -3927,17 +3992,21 @@
       <c r="AG18" s="40">
         <v>0.50549999999999995</v>
       </c>
-      <c r="AH18" s="44">
+      <c r="AH18" s="43">
         <v>115.8</v>
       </c>
-      <c r="AI18" s="44">
+      <c r="AI18" s="43">
         <v>87.8</v>
       </c>
-      <c r="AJ18" s="44">
+      <c r="AJ18" s="43">
         <v>81.599999999999994</v>
       </c>
-      <c r="AK18" s="33"/>
-      <c r="AL18" s="33"/>
+      <c r="AK18" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL18" s="45">
+        <v>104.8</v>
+      </c>
       <c r="AO18" s="8">
         <v>11.4</v>
       </c>
@@ -3952,7 +4021,7 @@
       </c>
     </row>
     <row r="19" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A19" s="42">
+      <c r="A19" s="41">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -4052,17 +4121,21 @@
       <c r="AG19" s="40">
         <v>0.54159999999999997</v>
       </c>
-      <c r="AH19" s="44">
+      <c r="AH19" s="43">
         <v>100.1</v>
       </c>
-      <c r="AI19" s="44">
+      <c r="AI19" s="43">
         <v>104.7</v>
       </c>
-      <c r="AJ19" s="44">
+      <c r="AJ19" s="43">
         <v>88.4</v>
       </c>
-      <c r="AK19" s="33"/>
-      <c r="AL19" s="33"/>
+      <c r="AK19" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL19" s="45">
+        <v>129.4</v>
+      </c>
       <c r="AO19" s="8">
         <v>13.7</v>
       </c>
@@ -4077,7 +4150,7 @@
       </c>
     </row>
     <row r="20" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A20" s="42">
+      <c r="A20" s="41">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -4177,17 +4250,21 @@
       <c r="AG20" s="40">
         <v>0.1331</v>
       </c>
-      <c r="AH20" s="44">
+      <c r="AH20" s="43">
         <v>31.672999999999998</v>
       </c>
-      <c r="AI20" s="44">
+      <c r="AI20" s="43">
         <v>32.045999999999999</v>
       </c>
-      <c r="AJ20" s="44">
+      <c r="AJ20" s="43">
         <v>27.34</v>
       </c>
-      <c r="AK20" s="33"/>
-      <c r="AL20" s="33"/>
+      <c r="AK20" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL20" s="45">
+        <v>168.6</v>
+      </c>
       <c r="AO20" s="8">
         <v>21.3</v>
       </c>
@@ -4202,7 +4279,7 @@
       </c>
     </row>
     <row r="21" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A21" s="42">
+      <c r="A21" s="41">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -4302,17 +4379,21 @@
       <c r="AG21" s="40">
         <v>0.13070000000000001</v>
       </c>
-      <c r="AH21" s="44">
+      <c r="AH21" s="43">
         <v>36.512999999999998</v>
       </c>
-      <c r="AI21" s="44">
+      <c r="AI21" s="43">
         <v>37.170999999999999</v>
       </c>
-      <c r="AJ21" s="44">
+      <c r="AJ21" s="43">
         <v>29.399000000000001</v>
       </c>
-      <c r="AK21" s="33"/>
-      <c r="AL21" s="33"/>
+      <c r="AK21" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL21" s="45">
+        <v>133</v>
+      </c>
       <c r="AO21" s="8">
         <v>18.399999999999999</v>
       </c>
@@ -4327,7 +4408,7 @@
       </c>
     </row>
     <row r="22" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A22" s="42">
+      <c r="A22" s="41">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -4427,17 +4508,21 @@
       <c r="AG22" s="40">
         <v>0.34</v>
       </c>
-      <c r="AH22" s="44">
+      <c r="AH22" s="43">
         <v>64.468000000000004</v>
       </c>
-      <c r="AI22" s="44">
+      <c r="AI22" s="43">
         <v>72.662999999999997</v>
       </c>
-      <c r="AJ22" s="44">
+      <c r="AJ22" s="43">
         <v>62.347000000000001</v>
       </c>
-      <c r="AK22" s="33"/>
-      <c r="AL22" s="33"/>
+      <c r="AK22" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL22" s="45">
+        <v>115.2</v>
+      </c>
       <c r="AO22" s="11">
         <v>9.6</v>
       </c>
@@ -4452,7 +4537,7 @@
       </c>
     </row>
     <row r="23" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A23" s="42">
+      <c r="A23" s="41">
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -4552,17 +4637,21 @@
       <c r="AG23" s="40">
         <v>0.7097</v>
       </c>
-      <c r="AH23" s="44">
+      <c r="AH23" s="43">
         <v>130.28700000000001</v>
       </c>
-      <c r="AI23" s="44">
+      <c r="AI23" s="43">
         <v>135.59800000000001</v>
       </c>
-      <c r="AJ23" s="44">
+      <c r="AJ23" s="43">
         <v>131.40799999999999</v>
       </c>
-      <c r="AK23" s="33"/>
-      <c r="AL23" s="33"/>
+      <c r="AK23" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL23" s="45">
+        <v>119</v>
+      </c>
       <c r="AO23" s="11">
         <v>11.8</v>
       </c>
@@ -4577,7 +4666,7 @@
       </c>
     </row>
     <row r="24" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A24" s="42">
+      <c r="A24" s="41">
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -4677,17 +4766,21 @@
       <c r="AG24" s="40">
         <v>0.1103</v>
       </c>
-      <c r="AH24" s="44">
+      <c r="AH24" s="43">
         <v>34.750999999999998</v>
       </c>
-      <c r="AI24" s="44">
+      <c r="AI24" s="43">
         <v>28.442</v>
       </c>
-      <c r="AJ24" s="44">
+      <c r="AJ24" s="43">
         <v>25.606000000000002</v>
       </c>
-      <c r="AK24" s="33"/>
-      <c r="AL24" s="33"/>
+      <c r="AK24" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL24" s="45">
+        <v>98.8</v>
+      </c>
       <c r="AO24" s="11">
         <v>12.3</v>
       </c>
@@ -4702,7 +4795,7 @@
       </c>
     </row>
     <row r="25" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A25" s="42">
+      <c r="A25" s="41">
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -4802,17 +4895,21 @@
       <c r="AG25" s="40">
         <v>0.19520000000000001</v>
       </c>
-      <c r="AH25" s="44">
+      <c r="AH25" s="43">
         <v>48.664000000000001</v>
       </c>
-      <c r="AI25" s="44">
+      <c r="AI25" s="43">
         <v>41.48</v>
       </c>
-      <c r="AJ25" s="44">
+      <c r="AJ25" s="43">
         <v>35.164000000000001</v>
       </c>
-      <c r="AK25" s="33"/>
-      <c r="AL25" s="33"/>
+      <c r="AK25" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL25" s="45">
+        <v>125.8</v>
+      </c>
       <c r="AO25" s="11">
         <v>21.1</v>
       </c>
@@ -4827,7 +4924,7 @@
       </c>
     </row>
     <row r="26" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A26" s="42">
+      <c r="A26" s="41">
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -4927,17 +5024,21 @@
       <c r="AG26" s="40">
         <v>0.29310000000000003</v>
       </c>
-      <c r="AH26" s="44">
+      <c r="AH26" s="43">
         <v>64.385999999999996</v>
       </c>
-      <c r="AI26" s="44">
+      <c r="AI26" s="43">
         <v>51.451999999999998</v>
       </c>
-      <c r="AJ26" s="44">
+      <c r="AJ26" s="43">
         <v>55.695999999999998</v>
       </c>
-      <c r="AK26" s="33"/>
-      <c r="AL26" s="33"/>
+      <c r="AK26" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL26" s="45">
+        <v>172.6</v>
+      </c>
       <c r="AO26" s="8">
         <v>16.2</v>
       </c>
@@ -4952,7 +5053,7 @@
       </c>
     </row>
     <row r="27" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A27" s="42">
+      <c r="A27" s="41">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -5052,17 +5153,21 @@
       <c r="AG27" s="40">
         <v>0.39279999999999998</v>
       </c>
-      <c r="AH27" s="44">
+      <c r="AH27" s="43">
         <v>101.402</v>
       </c>
-      <c r="AI27" s="44">
+      <c r="AI27" s="43">
         <v>82.090999999999994</v>
       </c>
-      <c r="AJ27" s="44">
+      <c r="AJ27" s="43">
         <v>68.584000000000003</v>
       </c>
-      <c r="AK27" s="33"/>
-      <c r="AL27" s="33"/>
+      <c r="AK27" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL27" s="45">
+        <v>170</v>
+      </c>
       <c r="AO27" s="8">
         <v>14</v>
       </c>
@@ -5077,7 +5182,7 @@
       </c>
     </row>
     <row r="28" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A28" s="42">
+      <c r="A28" s="41">
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -5177,17 +5282,21 @@
       <c r="AG28" s="40">
         <v>0.114</v>
       </c>
-      <c r="AH28" s="44">
+      <c r="AH28" s="43">
         <v>29.898</v>
       </c>
-      <c r="AI28" s="44">
+      <c r="AI28" s="43">
         <v>28.491</v>
       </c>
-      <c r="AJ28" s="44">
+      <c r="AJ28" s="43">
         <v>26.306999999999999</v>
       </c>
-      <c r="AK28" s="33"/>
-      <c r="AL28" s="33"/>
+      <c r="AK28" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL28" s="45">
+        <v>124</v>
+      </c>
       <c r="AO28" s="8">
         <v>17.5</v>
       </c>
@@ -5202,7 +5311,7 @@
       </c>
     </row>
     <row r="29" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A29" s="42">
+      <c r="A29" s="41">
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -5302,17 +5411,21 @@
       <c r="AG29" s="40">
         <v>0.152</v>
       </c>
-      <c r="AH29" s="44">
+      <c r="AH29" s="43">
         <v>45.253999999999998</v>
       </c>
-      <c r="AI29" s="44">
+      <c r="AI29" s="43">
         <v>35.508000000000003</v>
       </c>
-      <c r="AJ29" s="44">
+      <c r="AJ29" s="43">
         <v>25.54</v>
       </c>
-      <c r="AK29" s="33"/>
-      <c r="AL29" s="33"/>
+      <c r="AK29" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL29" s="45">
+        <v>116.2</v>
+      </c>
       <c r="AO29" s="8">
         <v>17.7</v>
       </c>
@@ -5327,7 +5440,7 @@
       </c>
     </row>
     <row r="30" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A30" s="42">
+      <c r="A30" s="41">
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -5427,17 +5540,21 @@
       <c r="AG30" s="40">
         <v>0.34670000000000001</v>
       </c>
-      <c r="AH30" s="44">
+      <c r="AH30" s="43">
         <v>130.31800000000001</v>
       </c>
-      <c r="AI30" s="44">
+      <c r="AI30" s="43">
         <v>113.691</v>
       </c>
-      <c r="AJ30" s="44">
+      <c r="AJ30" s="43">
         <v>52.252000000000002</v>
       </c>
-      <c r="AK30" s="33"/>
-      <c r="AL30" s="33"/>
+      <c r="AK30" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL30" s="45">
+        <v>158</v>
+      </c>
       <c r="AO30" s="8">
         <v>12</v>
       </c>
@@ -5452,7 +5569,7 @@
       </c>
     </row>
     <row r="31" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A31" s="42">
+      <c r="A31" s="41">
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -5552,14 +5669,20 @@
       <c r="AG31" s="40">
         <v>0.35759999999999997</v>
       </c>
-      <c r="AH31" s="44">
+      <c r="AH31" s="43">
         <v>68.753</v>
       </c>
-      <c r="AI31" s="44">
+      <c r="AI31" s="43">
         <v>62.320999999999998</v>
       </c>
-      <c r="AJ31" s="44">
+      <c r="AJ31" s="43">
         <v>56.499000000000002</v>
+      </c>
+      <c r="AK31" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL31" s="43">
+        <v>175.8</v>
       </c>
       <c r="AO31" s="8">
         <v>8.3000000000000007</v>
@@ -5575,7 +5698,7 @@
       </c>
     </row>
     <row r="32" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A32" s="42">
+      <c r="A32" s="41">
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -5675,17 +5798,21 @@
       <c r="AG32" s="40">
         <v>0.1205</v>
       </c>
-      <c r="AH32" s="44">
+      <c r="AH32" s="43">
         <v>30.204999999999998</v>
       </c>
-      <c r="AI32" s="44">
+      <c r="AI32" s="43">
         <v>27.600999999999999</v>
       </c>
-      <c r="AJ32" s="44">
+      <c r="AJ32" s="43">
         <v>22.626999999999999</v>
       </c>
-      <c r="AK32" s="33"/>
-      <c r="AL32" s="33"/>
+      <c r="AK32" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL32" s="45">
+        <v>125.2</v>
+      </c>
       <c r="AO32" s="8">
         <v>14.1</v>
       </c>
@@ -5700,7 +5827,7 @@
       </c>
     </row>
     <row r="33" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A33" s="42">
+      <c r="A33" s="41">
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -5800,17 +5927,21 @@
       <c r="AG33" s="40">
         <v>0.2155</v>
       </c>
-      <c r="AH33" s="44">
+      <c r="AH33" s="43">
         <v>72.513000000000005</v>
       </c>
-      <c r="AI33" s="44">
+      <c r="AI33" s="43">
         <v>57.945999999999998</v>
       </c>
-      <c r="AJ33" s="44">
+      <c r="AJ33" s="43">
         <v>37.679000000000002</v>
       </c>
-      <c r="AK33" s="33"/>
-      <c r="AL33" s="33"/>
+      <c r="AK33" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL33" s="45">
+        <v>153.19999999999999</v>
+      </c>
       <c r="AO33" s="8">
         <v>16.399999999999999</v>
       </c>
@@ -5825,7 +5956,7 @@
       </c>
     </row>
     <row r="34" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A34" s="42">
+      <c r="A34" s="41">
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -5925,17 +6056,21 @@
       <c r="AG34" s="40">
         <v>0.39529999999999998</v>
       </c>
-      <c r="AH34" s="44">
+      <c r="AH34" s="43">
         <v>100.621</v>
       </c>
-      <c r="AI34" s="44">
+      <c r="AI34" s="43">
         <v>92.203000000000003</v>
       </c>
-      <c r="AJ34" s="44">
+      <c r="AJ34" s="43">
         <v>66.929000000000002</v>
       </c>
-      <c r="AK34" s="33"/>
-      <c r="AL34" s="33"/>
+      <c r="AK34" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL34" s="45">
+        <v>99</v>
+      </c>
       <c r="AO34" s="8">
         <v>12.7</v>
       </c>
@@ -5950,7 +6085,7 @@
       </c>
     </row>
     <row r="35" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A35" s="42">
+      <c r="A35" s="41">
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -6050,17 +6185,21 @@
       <c r="AG35" s="40">
         <v>0.47760000000000002</v>
       </c>
-      <c r="AH35" s="44">
+      <c r="AH35" s="43">
         <v>122.321</v>
       </c>
-      <c r="AI35" s="44">
+      <c r="AI35" s="43">
         <v>120.785</v>
       </c>
-      <c r="AJ35" s="44">
+      <c r="AJ35" s="43">
         <v>95.195999999999998</v>
       </c>
-      <c r="AK35" s="33"/>
-      <c r="AL35" s="33"/>
+      <c r="AK35" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL35" s="45">
+        <v>97</v>
+      </c>
       <c r="AO35" s="8">
         <v>13.1</v>
       </c>
@@ -6075,7 +6214,7 @@
       </c>
     </row>
     <row r="36" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A36" s="42">
+      <c r="A36" s="41">
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
@@ -6175,17 +6314,21 @@
       <c r="AG36" s="40">
         <v>8.5199999999999998E-2</v>
       </c>
-      <c r="AH36" s="44">
+      <c r="AH36" s="43">
         <v>42.173000000000002</v>
       </c>
-      <c r="AI36" s="45">
+      <c r="AI36" s="44">
         <v>19.739999999999998</v>
       </c>
-      <c r="AJ36" s="45">
+      <c r="AJ36" s="44">
         <v>19.959</v>
       </c>
-      <c r="AK36" s="33"/>
-      <c r="AL36" s="33"/>
+      <c r="AK36" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL36" s="45">
+        <v>102.2</v>
+      </c>
       <c r="AO36" s="8">
         <v>15.6</v>
       </c>
@@ -6200,7 +6343,7 @@
       </c>
     </row>
     <row r="37" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A37" s="42">
+      <c r="A37" s="41">
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
@@ -6300,17 +6443,21 @@
       <c r="AG37" s="40">
         <v>0.1186</v>
       </c>
-      <c r="AH37" s="45">
+      <c r="AH37" s="44">
         <v>37.588999999999999</v>
       </c>
-      <c r="AI37" s="45">
+      <c r="AI37" s="44">
         <v>29.776</v>
       </c>
-      <c r="AJ37" s="45">
+      <c r="AJ37" s="44">
         <v>25.673999999999999</v>
       </c>
-      <c r="AK37" s="33"/>
-      <c r="AL37" s="33"/>
+      <c r="AK37" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL37" s="45">
+        <v>88.8</v>
+      </c>
       <c r="AO37" s="8">
         <v>13</v>
       </c>
@@ -6325,7 +6472,7 @@
       </c>
     </row>
     <row r="38" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A38" s="42">
+      <c r="A38" s="41">
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -6425,17 +6572,21 @@
       <c r="AG38" s="40">
         <v>0.57909999999999995</v>
       </c>
-      <c r="AH38" s="45">
+      <c r="AH38" s="44">
         <v>197.64400000000001</v>
       </c>
-      <c r="AI38" s="45">
+      <c r="AI38" s="44">
         <v>143.47499999999999</v>
       </c>
-      <c r="AJ38" s="45">
+      <c r="AJ38" s="44">
         <v>109.501</v>
       </c>
-      <c r="AK38" s="33"/>
-      <c r="AL38" s="33"/>
+      <c r="AK38" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL38" s="45">
+        <v>132.6</v>
+      </c>
       <c r="AO38" s="8">
         <v>17.2</v>
       </c>
@@ -6450,7 +6601,7 @@
       </c>
     </row>
     <row r="39" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A39" s="42">
+      <c r="A39" s="41">
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
@@ -6550,17 +6701,21 @@
       <c r="AG39" s="40">
         <v>0.40810000000000002</v>
       </c>
-      <c r="AH39" s="45">
+      <c r="AH39" s="44">
         <v>111.59699999999999</v>
       </c>
-      <c r="AI39" s="45">
+      <c r="AI39" s="44">
         <v>104.816</v>
       </c>
-      <c r="AJ39" s="45">
+      <c r="AJ39" s="44">
         <v>78.293000000000006</v>
       </c>
-      <c r="AK39" s="33"/>
-      <c r="AL39" s="33"/>
+      <c r="AK39" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL39" s="45">
+        <v>126</v>
+      </c>
       <c r="AO39" s="8">
         <v>12</v>
       </c>
@@ -6575,7 +6730,7 @@
       </c>
     </row>
     <row r="40" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A40" s="42">
+      <c r="A40" s="41">
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
@@ -6675,17 +6830,21 @@
       <c r="AG40" s="40">
         <v>0.21210000000000001</v>
       </c>
-      <c r="AH40" s="45">
+      <c r="AH40" s="44">
         <v>44.4</v>
       </c>
-      <c r="AI40" s="45">
+      <c r="AI40" s="44">
         <v>34.496000000000002</v>
       </c>
-      <c r="AJ40" s="45">
+      <c r="AJ40" s="44">
         <v>34.545999999999999</v>
       </c>
-      <c r="AK40" s="33"/>
-      <c r="AL40" s="33"/>
+      <c r="AK40" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL40" s="45">
+        <v>133.6</v>
+      </c>
       <c r="AO40" s="8">
         <v>15.3</v>
       </c>
@@ -6700,7 +6859,7 @@
       </c>
     </row>
     <row r="41" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A41" s="42">
+      <c r="A41" s="41">
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
@@ -6800,17 +6959,21 @@
       <c r="AG41" s="40">
         <v>0.15959999999999999</v>
       </c>
-      <c r="AH41" s="45">
+      <c r="AH41" s="44">
         <v>50.372</v>
       </c>
-      <c r="AI41" s="45">
+      <c r="AI41" s="44">
         <v>50.703000000000003</v>
       </c>
-      <c r="AJ41" s="45">
+      <c r="AJ41" s="44">
         <v>32.387</v>
       </c>
-      <c r="AK41" s="33"/>
-      <c r="AL41" s="33"/>
+      <c r="AK41" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL41" s="45">
+        <v>113.8</v>
+      </c>
       <c r="AO41" s="8">
         <v>16.100000000000001</v>
       </c>
@@ -6825,7 +6988,7 @@
       </c>
     </row>
     <row r="42" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A42" s="42">
+      <c r="A42" s="41">
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
@@ -6925,17 +7088,21 @@
       <c r="AG42" s="40">
         <v>0.44629999999999997</v>
       </c>
-      <c r="AH42" s="45">
+      <c r="AH42" s="44">
         <v>92.600999999999999</v>
       </c>
-      <c r="AI42" s="45">
+      <c r="AI42" s="44">
         <v>74.811000000000007</v>
       </c>
-      <c r="AJ42" s="45">
+      <c r="AJ42" s="44">
         <v>68.155000000000001</v>
       </c>
-      <c r="AK42" s="33"/>
-      <c r="AL42" s="33"/>
+      <c r="AK42" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL42" s="45">
+        <v>206.8</v>
+      </c>
       <c r="AO42" s="2">
         <v>17</v>
       </c>
@@ -6951,7 +7118,7 @@
       <c r="AS42" s="11"/>
     </row>
     <row r="43" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A43" s="42">
+      <c r="A43" s="41">
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
@@ -7051,17 +7218,21 @@
       <c r="AG43" s="40">
         <v>0.45910000000000001</v>
       </c>
-      <c r="AH43" s="45">
+      <c r="AH43" s="44">
         <v>81.646000000000001</v>
       </c>
-      <c r="AI43" s="45">
+      <c r="AI43" s="44">
         <v>91.956000000000003</v>
       </c>
-      <c r="AJ43" s="45">
+      <c r="AJ43" s="44">
         <v>84.414000000000001</v>
       </c>
-      <c r="AK43" s="33"/>
-      <c r="AL43" s="33"/>
+      <c r="AK43" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL43" s="45">
+        <v>97.8</v>
+      </c>
       <c r="AO43" s="2">
         <v>18.5</v>
       </c>
@@ -7077,7 +7248,7 @@
       <c r="AS43" s="11"/>
     </row>
     <row r="44" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A44" s="42">
+      <c r="A44" s="41">
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
@@ -7177,17 +7348,21 @@
       <c r="AG44" s="40">
         <v>0.1192</v>
       </c>
-      <c r="AH44" s="45">
+      <c r="AH44" s="44">
         <v>37.095999999999997</v>
       </c>
-      <c r="AI44" s="45">
+      <c r="AI44" s="44">
         <v>34.246000000000002</v>
       </c>
-      <c r="AJ44" s="45">
+      <c r="AJ44" s="44">
         <v>28.062999999999999</v>
       </c>
-      <c r="AK44" s="33"/>
-      <c r="AL44" s="33"/>
+      <c r="AK44" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL44" s="45">
+        <v>184.6</v>
+      </c>
       <c r="AO44" s="2">
         <v>21.4</v>
       </c>
@@ -7203,7 +7378,7 @@
       <c r="AS44" s="11"/>
     </row>
     <row r="45" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A45" s="42">
+      <c r="A45" s="41">
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
@@ -7303,17 +7478,21 @@
       <c r="AG45" s="40">
         <v>7.3599999999999999E-2</v>
       </c>
-      <c r="AH45" s="45">
+      <c r="AH45" s="44">
         <v>22.076000000000001</v>
       </c>
-      <c r="AI45" s="45">
+      <c r="AI45" s="44">
         <v>22.105</v>
       </c>
-      <c r="AJ45" s="45">
+      <c r="AJ45" s="44">
         <v>18.684000000000001</v>
       </c>
-      <c r="AK45" s="33"/>
-      <c r="AL45" s="33"/>
+      <c r="AK45" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL45" s="45">
+        <v>84</v>
+      </c>
       <c r="AO45" s="2">
         <v>12.9</v>
       </c>
@@ -7329,7 +7508,7 @@
       <c r="AS45" s="11"/>
     </row>
     <row r="46" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A46" s="42">
+      <c r="A46" s="41">
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
@@ -7429,14 +7608,20 @@
       <c r="AG46" s="40">
         <v>0.41959999999999997</v>
       </c>
-      <c r="AH46" s="45">
+      <c r="AH46" s="44">
         <v>85.507000000000005</v>
       </c>
-      <c r="AI46" s="45">
+      <c r="AI46" s="44">
         <v>59.445999999999998</v>
       </c>
-      <c r="AJ46" s="45">
+      <c r="AJ46" s="44">
         <v>65.986000000000004</v>
+      </c>
+      <c r="AK46" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL46" s="45">
+        <v>184.8</v>
       </c>
       <c r="AO46" s="8">
         <v>17.399999999999999</v>
@@ -7452,7 +7637,7 @@
       </c>
     </row>
     <row r="47" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A47" s="42">
+      <c r="A47" s="41">
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
@@ -7552,17 +7737,21 @@
       <c r="AG47" s="40">
         <v>0.38100000000000001</v>
       </c>
-      <c r="AH47" s="45">
+      <c r="AH47" s="44">
         <v>115.148</v>
       </c>
-      <c r="AI47" s="45">
+      <c r="AI47" s="44">
         <v>112.43300000000001</v>
       </c>
-      <c r="AJ47" s="45">
+      <c r="AJ47" s="44">
         <v>63.506</v>
       </c>
-      <c r="AK47" s="33"/>
-      <c r="AL47" s="33"/>
+      <c r="AK47" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL47" s="45">
+        <v>75.8</v>
+      </c>
       <c r="AO47" s="8">
         <v>8.5</v>
       </c>
@@ -7577,7 +7766,7 @@
       </c>
     </row>
     <row r="48" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A48" s="42">
+      <c r="A48" s="41">
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
@@ -7677,17 +7866,21 @@
       <c r="AG48" s="40">
         <v>0.1686</v>
       </c>
-      <c r="AH48" s="45">
+      <c r="AH48" s="44">
         <v>41.786000000000001</v>
       </c>
-      <c r="AI48" s="45">
+      <c r="AI48" s="44">
         <v>34.683999999999997</v>
       </c>
-      <c r="AJ48" s="45">
+      <c r="AJ48" s="44">
         <v>29.463000000000001</v>
       </c>
-      <c r="AK48" s="33"/>
-      <c r="AL48" s="33"/>
+      <c r="AK48" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL48" s="45">
+        <v>119.2</v>
+      </c>
       <c r="AO48" s="8">
         <v>18.100000000000001</v>
       </c>
@@ -7702,7 +7895,7 @@
       </c>
     </row>
     <row r="49" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A49" s="42">
+      <c r="A49" s="41">
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
@@ -7802,17 +7995,21 @@
       <c r="AG49" s="40">
         <v>8.43E-2</v>
       </c>
-      <c r="AH49" s="44">
+      <c r="AH49" s="43">
         <v>18.05</v>
       </c>
-      <c r="AI49" s="44">
+      <c r="AI49" s="43">
         <v>30.12</v>
       </c>
-      <c r="AJ49" s="45">
+      <c r="AJ49" s="44">
         <v>17.940000000000001</v>
       </c>
-      <c r="AK49" s="33"/>
-      <c r="AL49" s="33"/>
+      <c r="AK49" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL49" s="45">
+        <v>92.6</v>
+      </c>
       <c r="AO49" s="8">
         <v>11.8</v>
       </c>
@@ -7827,7 +8024,7 @@
       </c>
     </row>
     <row r="50" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A50" s="42">
+      <c r="A50" s="41">
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
@@ -7927,17 +8124,21 @@
       <c r="AG50" s="40">
         <v>0.37359999999999999</v>
       </c>
-      <c r="AH50" s="44">
+      <c r="AH50" s="43">
         <v>126.902</v>
       </c>
-      <c r="AI50" s="44">
+      <c r="AI50" s="43">
         <v>95.926000000000002</v>
       </c>
-      <c r="AJ50" s="45">
+      <c r="AJ50" s="44">
         <v>65.415999999999997</v>
       </c>
-      <c r="AK50" s="33"/>
-      <c r="AL50" s="33"/>
+      <c r="AK50" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL50" s="45">
+        <v>93.6</v>
+      </c>
       <c r="AO50" s="8">
         <v>9.9</v>
       </c>
@@ -7952,7 +8153,7 @@
       </c>
     </row>
     <row r="51" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A51" s="42">
+      <c r="A51" s="41">
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
@@ -8052,17 +8253,21 @@
       <c r="AG51" s="40">
         <v>0.38800000000000001</v>
       </c>
-      <c r="AH51" s="45">
+      <c r="AH51" s="44">
         <v>115.066</v>
       </c>
-      <c r="AI51" s="45">
+      <c r="AI51" s="44">
         <v>76.451999999999998</v>
       </c>
-      <c r="AJ51" s="45">
+      <c r="AJ51" s="44">
         <v>74.355999999999995</v>
       </c>
-      <c r="AK51" s="33"/>
-      <c r="AL51" s="33"/>
+      <c r="AK51" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL51" s="45">
+        <v>105.8</v>
+      </c>
       <c r="AO51" s="8">
         <v>8.6999999999999993</v>
       </c>
@@ -8077,7 +8282,7 @@
       </c>
     </row>
     <row r="52" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A52" s="42">
+      <c r="A52" s="41">
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
@@ -8177,17 +8382,21 @@
       <c r="AG52" s="40">
         <v>0.13600000000000001</v>
       </c>
-      <c r="AH52" s="45">
+      <c r="AH52" s="44">
         <v>30.92</v>
       </c>
-      <c r="AI52" s="45">
+      <c r="AI52" s="44">
         <v>29.898</v>
       </c>
-      <c r="AJ52" s="45">
+      <c r="AJ52" s="44">
         <v>23.431999999999999</v>
       </c>
-      <c r="AK52" s="33"/>
-      <c r="AL52" s="33"/>
+      <c r="AK52" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL52" s="45">
+        <v>141.80000000000001</v>
+      </c>
       <c r="AO52" s="8">
         <v>15</v>
       </c>
@@ -8202,7 +8411,7 @@
       </c>
     </row>
     <row r="53" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A53" s="42">
+      <c r="A53" s="41">
         <v>52</v>
       </c>
       <c r="B53" s="2" t="s">
@@ -8302,17 +8511,21 @@
       <c r="AG53" s="40">
         <v>0.13200000000000001</v>
       </c>
-      <c r="AH53" s="45">
+      <c r="AH53" s="44">
         <v>26.355</v>
       </c>
-      <c r="AI53" s="45">
+      <c r="AI53" s="44">
         <v>21.802</v>
       </c>
-      <c r="AJ53" s="45">
+      <c r="AJ53" s="44">
         <v>24.87</v>
       </c>
-      <c r="AK53" s="33"/>
-      <c r="AL53" s="33"/>
+      <c r="AK53" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL53" s="45">
+        <v>151.80000000000001</v>
+      </c>
       <c r="AO53" s="8">
         <v>14.6</v>
       </c>
@@ -8327,7 +8540,7 @@
       </c>
     </row>
     <row r="54" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A54" s="42">
+      <c r="A54" s="41">
         <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
@@ -8427,17 +8640,21 @@
       <c r="AG54" s="40">
         <v>0.29210000000000003</v>
       </c>
-      <c r="AH54" s="45">
+      <c r="AH54" s="44">
         <v>71.001999999999995</v>
       </c>
-      <c r="AI54" s="45">
+      <c r="AI54" s="44">
         <v>57.728000000000002</v>
       </c>
-      <c r="AJ54" s="45">
+      <c r="AJ54" s="44">
         <v>44</v>
       </c>
-      <c r="AK54" s="33"/>
-      <c r="AL54" s="33"/>
+      <c r="AK54" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL54" s="45">
+        <v>140.80000000000001</v>
+      </c>
       <c r="AO54" s="8">
         <v>14</v>
       </c>
@@ -8452,7 +8669,7 @@
       </c>
     </row>
     <row r="55" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A55" s="42">
+      <c r="A55" s="41">
         <v>54</v>
       </c>
       <c r="B55" s="2" t="s">
@@ -8552,14 +8769,20 @@
       <c r="AG55" s="40">
         <v>0.32269999999999999</v>
       </c>
-      <c r="AH55" s="45">
+      <c r="AH55" s="44">
         <v>85.513999999999996</v>
       </c>
-      <c r="AI55" s="45">
+      <c r="AI55" s="44">
         <v>76.129000000000005</v>
       </c>
-      <c r="AJ55" s="45">
+      <c r="AJ55" s="44">
         <v>57.271999999999998</v>
+      </c>
+      <c r="AK55" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL55" s="44">
+        <v>113.4</v>
       </c>
       <c r="AO55" s="8">
         <v>14.4</v>
@@ -8575,7 +8798,7 @@
       </c>
     </row>
     <row r="56" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A56" s="42">
+      <c r="A56" s="41">
         <v>55</v>
       </c>
       <c r="B56" s="2" t="s">
@@ -8675,14 +8898,20 @@
       <c r="AG56" s="40">
         <v>0.15029999999999999</v>
       </c>
-      <c r="AH56" s="45">
+      <c r="AH56" s="44">
         <v>35.685000000000002</v>
       </c>
-      <c r="AI56" s="45">
+      <c r="AI56" s="44">
         <v>34.671999999999997</v>
       </c>
-      <c r="AJ56" s="45">
+      <c r="AJ56" s="44">
         <v>32.438000000000002</v>
+      </c>
+      <c r="AK56" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL56" s="45">
+        <v>119</v>
       </c>
       <c r="AO56" s="8">
         <v>16.899999999999999</v>
@@ -8698,7 +8927,7 @@
       </c>
     </row>
     <row r="57" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A57" s="42">
+      <c r="A57" s="41">
         <v>56</v>
       </c>
       <c r="B57" s="2" t="s">
@@ -8798,14 +9027,20 @@
       <c r="AG57" s="40">
         <v>8.6800000000000002E-2</v>
       </c>
-      <c r="AH57" s="45">
+      <c r="AH57" s="44">
         <v>27.841000000000001</v>
       </c>
-      <c r="AI57" s="45">
+      <c r="AI57" s="44">
         <v>20.295000000000002</v>
       </c>
-      <c r="AJ57" s="45">
+      <c r="AJ57" s="44">
         <v>17.21</v>
+      </c>
+      <c r="AK57" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL57" s="44">
+        <v>99.6</v>
       </c>
       <c r="AO57" s="8">
         <v>17</v>
@@ -8821,7 +9056,7 @@
       </c>
     </row>
     <row r="58" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A58" s="42">
+      <c r="A58" s="41">
         <v>57</v>
       </c>
       <c r="B58" s="2" t="s">
@@ -8921,14 +9156,20 @@
       <c r="AG58" s="40">
         <v>0.38590000000000002</v>
       </c>
-      <c r="AH58" s="45">
+      <c r="AH58" s="44">
         <v>76.763000000000005</v>
       </c>
-      <c r="AI58" s="45">
+      <c r="AI58" s="44">
         <v>67.210999999999999</v>
       </c>
-      <c r="AJ58" s="45">
+      <c r="AJ58" s="44">
         <v>70.742000000000004</v>
+      </c>
+      <c r="AK58" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL58" s="45">
+        <v>98.6</v>
       </c>
       <c r="AO58" s="8">
         <v>11.6</v>
@@ -8944,7 +9185,7 @@
       </c>
     </row>
     <row r="59" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A59" s="42">
+      <c r="A59" s="41">
         <v>58</v>
       </c>
       <c r="B59" s="2" t="s">
@@ -9044,17 +9285,21 @@
       <c r="AG59" s="40">
         <v>0.36780000000000002</v>
       </c>
-      <c r="AH59" s="45">
+      <c r="AH59" s="44">
         <v>62.155999999999999</v>
       </c>
-      <c r="AI59" s="45">
+      <c r="AI59" s="44">
         <v>64.087000000000003</v>
       </c>
-      <c r="AJ59" s="45">
+      <c r="AJ59" s="44">
         <v>60.356999999999999</v>
       </c>
-      <c r="AK59" s="33"/>
-      <c r="AL59" s="33"/>
+      <c r="AK59" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL59" s="45">
+        <v>104.4</v>
+      </c>
       <c r="AO59" s="8">
         <v>14.2</v>
       </c>
@@ -9069,7 +9314,7 @@
       </c>
     </row>
     <row r="60" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A60" s="42">
+      <c r="A60" s="41">
         <v>59</v>
       </c>
       <c r="B60" s="2" t="s">
@@ -9169,17 +9414,21 @@
       <c r="AG60" s="40">
         <v>0.1132</v>
       </c>
-      <c r="AH60" s="45">
+      <c r="AH60" s="44">
         <v>30.427</v>
       </c>
-      <c r="AI60" s="45">
+      <c r="AI60" s="44">
         <v>26.134</v>
       </c>
-      <c r="AJ60" s="45">
+      <c r="AJ60" s="44">
         <v>23.756</v>
       </c>
-      <c r="AK60" s="33"/>
-      <c r="AL60" s="33"/>
+      <c r="AK60" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL60" s="45">
+        <v>141.4</v>
+      </c>
       <c r="AO60" s="8">
         <v>17</v>
       </c>
@@ -9194,7 +9443,7 @@
       </c>
     </row>
     <row r="61" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A61" s="42">
+      <c r="A61" s="41">
         <v>60</v>
       </c>
       <c r="B61" s="2" t="s">
@@ -9294,17 +9543,21 @@
       <c r="AG61" s="40">
         <v>9.4100000000000003E-2</v>
       </c>
-      <c r="AH61" s="45">
+      <c r="AH61" s="44">
         <v>23.968</v>
       </c>
-      <c r="AI61" s="45">
+      <c r="AI61" s="44">
         <v>19.771000000000001</v>
       </c>
-      <c r="AJ61" s="45">
+      <c r="AJ61" s="44">
         <v>18.239999999999998</v>
       </c>
-      <c r="AK61" s="33"/>
-      <c r="AL61" s="33"/>
+      <c r="AK61" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL61" s="45">
+        <v>78.2</v>
+      </c>
       <c r="AO61" s="8">
         <v>12.9</v>
       </c>
@@ -9319,7 +9572,7 @@
       </c>
     </row>
     <row r="62" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A62" s="42">
+      <c r="A62" s="41">
         <v>61</v>
       </c>
       <c r="B62" s="2" t="s">
@@ -9419,17 +9672,21 @@
       <c r="AG62" s="40">
         <v>0.41660000000000003</v>
       </c>
-      <c r="AH62" s="45">
+      <c r="AH62" s="44">
         <v>99.367999999999995</v>
       </c>
-      <c r="AI62" s="45">
+      <c r="AI62" s="44">
         <v>91.602000000000004</v>
       </c>
-      <c r="AJ62" s="45">
+      <c r="AJ62" s="44">
         <v>82.691000000000003</v>
       </c>
-      <c r="AK62" s="33"/>
-      <c r="AL62" s="33"/>
+      <c r="AK62" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL62" s="45">
+        <v>80.599999999999994</v>
+      </c>
       <c r="AO62" s="11">
         <v>10.1</v>
       </c>
@@ -9444,7 +9701,7 @@
       </c>
     </row>
     <row r="63" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A63" s="42">
+      <c r="A63" s="41">
         <v>62</v>
       </c>
       <c r="B63" s="2" t="s">
@@ -9544,17 +9801,21 @@
       <c r="AG63" s="40">
         <v>0.52610000000000001</v>
       </c>
-      <c r="AH63" s="45">
+      <c r="AH63" s="44">
         <v>89.554000000000002</v>
       </c>
-      <c r="AI63" s="45">
+      <c r="AI63" s="44">
         <v>86.174000000000007</v>
       </c>
-      <c r="AJ63" s="45">
+      <c r="AJ63" s="44">
         <v>82.628</v>
       </c>
-      <c r="AK63" s="33"/>
-      <c r="AL63" s="33"/>
+      <c r="AK63" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL63" s="45">
+        <v>138.80000000000001</v>
+      </c>
       <c r="AO63" s="8">
         <v>18.7</v>
       </c>
@@ -9569,7 +9830,7 @@
       </c>
     </row>
     <row r="64" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A64" s="42">
+      <c r="A64" s="41">
         <v>63</v>
       </c>
       <c r="B64" s="2" t="s">
@@ -9669,17 +9930,21 @@
       <c r="AG64" s="40">
         <v>0.11260000000000001</v>
       </c>
-      <c r="AH64" s="45">
+      <c r="AH64" s="44">
         <v>29.902999999999999</v>
       </c>
-      <c r="AI64" s="45">
+      <c r="AI64" s="44">
         <v>21.306000000000001</v>
       </c>
-      <c r="AJ64" s="45">
+      <c r="AJ64" s="44">
         <v>22.579000000000001</v>
       </c>
-      <c r="AK64" s="33"/>
-      <c r="AL64" s="33"/>
+      <c r="AK64" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL64" s="45">
+        <v>79.400000000000006</v>
+      </c>
       <c r="AO64" s="8">
         <v>14.6</v>
       </c>
@@ -9694,7 +9959,7 @@
       </c>
     </row>
     <row r="65" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A65" s="42">
+      <c r="A65" s="41">
         <v>64</v>
       </c>
       <c r="B65" s="2" t="s">
@@ -9794,17 +10059,21 @@
       <c r="AG65" s="40">
         <v>0.14430000000000001</v>
       </c>
-      <c r="AH65" s="45">
+      <c r="AH65" s="44">
         <v>40.773000000000003</v>
       </c>
-      <c r="AI65" s="45">
+      <c r="AI65" s="44">
         <v>35.305</v>
       </c>
-      <c r="AJ65" s="45">
+      <c r="AJ65" s="44">
         <v>31.030999999999999</v>
       </c>
-      <c r="AK65" s="33"/>
-      <c r="AL65" s="33"/>
+      <c r="AK65" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL65" s="45">
+        <v>70.8</v>
+      </c>
       <c r="AO65" s="8">
         <v>16.399999999999999</v>
       </c>
@@ -9819,7 +10088,7 @@
       </c>
     </row>
     <row r="66" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A66" s="42">
+      <c r="A66" s="41">
         <v>65</v>
       </c>
       <c r="B66" s="2" t="s">
@@ -9919,17 +10188,21 @@
       <c r="AG66" s="40">
         <v>0.51180000000000003</v>
       </c>
-      <c r="AH66" s="45">
+      <c r="AH66" s="44">
         <v>90.051000000000002</v>
       </c>
-      <c r="AI66" s="45">
+      <c r="AI66" s="44">
         <v>86.664000000000001</v>
       </c>
-      <c r="AJ66" s="45">
+      <c r="AJ66" s="44">
         <v>81.819000000000003</v>
       </c>
-      <c r="AK66" s="33"/>
-      <c r="AL66" s="33"/>
+      <c r="AK66" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL66" s="45">
+        <v>104.4</v>
+      </c>
       <c r="AO66" s="8">
         <v>9.1</v>
       </c>
@@ -9944,7 +10217,7 @@
       </c>
     </row>
     <row r="67" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A67" s="42">
+      <c r="A67" s="41">
         <v>66</v>
       </c>
       <c r="B67" s="2" t="s">
@@ -10044,17 +10317,21 @@
       <c r="AG67" s="40">
         <v>0.68479999999999996</v>
       </c>
-      <c r="AH67" s="45">
+      <c r="AH67" s="44">
         <v>83.05</v>
       </c>
-      <c r="AI67" s="45">
+      <c r="AI67" s="44">
         <v>95.147000000000006</v>
       </c>
-      <c r="AJ67" s="45">
+      <c r="AJ67" s="44">
         <v>110.011</v>
       </c>
-      <c r="AK67" s="33"/>
-      <c r="AL67" s="33"/>
+      <c r="AK67" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL67" s="45">
+        <v>100.4</v>
+      </c>
       <c r="AO67" s="8">
         <v>10</v>
       </c>
@@ -10069,7 +10346,7 @@
       </c>
     </row>
     <row r="68" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A68" s="42">
+      <c r="A68" s="41">
         <v>67</v>
       </c>
       <c r="B68" s="2" t="s">
@@ -10169,17 +10446,21 @@
       <c r="AG68" s="40">
         <v>8.3299999999999999E-2</v>
       </c>
-      <c r="AH68" s="45">
+      <c r="AH68" s="44">
         <v>25.716999999999999</v>
       </c>
-      <c r="AI68" s="45">
+      <c r="AI68" s="44">
         <v>17.309999999999999</v>
       </c>
-      <c r="AJ68" s="45">
+      <c r="AJ68" s="44">
         <v>14.441000000000001</v>
       </c>
-      <c r="AK68" s="33"/>
-      <c r="AL68" s="33"/>
+      <c r="AK68" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL68" s="45">
+        <v>95.8</v>
+      </c>
       <c r="AO68" s="8">
         <v>16.8</v>
       </c>
@@ -10194,7 +10475,7 @@
       </c>
     </row>
     <row r="69" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A69" s="42">
+      <c r="A69" s="41">
         <v>68</v>
       </c>
       <c r="B69" s="2" t="s">
@@ -10294,14 +10575,20 @@
       <c r="AG69" s="40">
         <v>0.11360000000000001</v>
       </c>
-      <c r="AH69" s="45">
+      <c r="AH69" s="44">
         <v>22.530999999999999</v>
       </c>
-      <c r="AI69" s="45">
+      <c r="AI69" s="44">
         <v>21.529</v>
       </c>
-      <c r="AJ69" s="45">
+      <c r="AJ69" s="44">
         <v>22.027000000000001</v>
+      </c>
+      <c r="AK69" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL69" s="45">
+        <v>111</v>
       </c>
       <c r="AO69" s="8">
         <v>18.600000000000001</v>
@@ -10317,7 +10604,7 @@
       </c>
     </row>
     <row r="70" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A70" s="42">
+      <c r="A70" s="41">
         <v>69</v>
       </c>
       <c r="B70" s="2" t="s">
@@ -10417,17 +10704,21 @@
       <c r="AG70" s="40">
         <v>0.56379999999999997</v>
       </c>
-      <c r="AH70" s="45">
+      <c r="AH70" s="44">
         <v>96.188000000000002</v>
       </c>
-      <c r="AI70" s="45">
+      <c r="AI70" s="44">
         <v>54.75</v>
       </c>
-      <c r="AJ70" s="45">
+      <c r="AJ70" s="44">
         <v>96.8</v>
       </c>
-      <c r="AK70" s="33"/>
-      <c r="AL70" s="33"/>
+      <c r="AK70" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL70" s="45">
+        <v>78.400000000000006</v>
+      </c>
       <c r="AO70" s="8">
         <v>10.1</v>
       </c>
@@ -10442,7 +10733,7 @@
       </c>
     </row>
     <row r="71" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A71" s="42">
+      <c r="A71" s="41">
         <v>70</v>
       </c>
       <c r="B71" s="2" t="s">
@@ -10542,17 +10833,21 @@
       <c r="AG71" s="40">
         <v>0.56979999999999997</v>
       </c>
-      <c r="AH71" s="45">
+      <c r="AH71" s="44">
         <v>78.712999999999994</v>
       </c>
-      <c r="AI71" s="45">
+      <c r="AI71" s="44">
         <v>88.44</v>
       </c>
-      <c r="AJ71" s="45">
+      <c r="AJ71" s="44">
         <v>76.744</v>
       </c>
-      <c r="AK71" s="33"/>
-      <c r="AL71" s="33"/>
+      <c r="AK71" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL71" s="45">
+        <v>155</v>
+      </c>
       <c r="AO71" s="8">
         <v>13.4</v>
       </c>
@@ -10567,7 +10862,7 @@
       </c>
     </row>
     <row r="72" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A72" s="42">
+      <c r="A72" s="41">
         <v>71</v>
       </c>
       <c r="B72" s="2" t="s">
@@ -10667,17 +10962,21 @@
       <c r="AG72" s="40">
         <v>9.6699999999999994E-2</v>
       </c>
-      <c r="AH72" s="45">
+      <c r="AH72" s="44">
         <v>21.437000000000001</v>
       </c>
-      <c r="AI72" s="45">
+      <c r="AI72" s="44">
         <v>22.196000000000002</v>
       </c>
-      <c r="AJ72" s="45">
+      <c r="AJ72" s="44">
         <v>17.741</v>
       </c>
-      <c r="AK72" s="33"/>
-      <c r="AL72" s="33"/>
+      <c r="AK72" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL72" s="45">
+        <v>89.4</v>
+      </c>
       <c r="AO72" s="8">
         <v>15.6</v>
       </c>
@@ -10692,7 +10991,7 @@
       </c>
     </row>
     <row r="73" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A73" s="42">
+      <c r="A73" s="41">
         <v>72</v>
       </c>
       <c r="B73" s="2" t="s">
@@ -10792,17 +11091,21 @@
       <c r="AG73" s="40">
         <v>8.9200000000000002E-2</v>
       </c>
-      <c r="AH73" s="45">
+      <c r="AH73" s="44">
         <v>23.486999999999998</v>
       </c>
-      <c r="AI73" s="45">
+      <c r="AI73" s="44">
         <v>19.077000000000002</v>
       </c>
-      <c r="AJ73" s="45">
+      <c r="AJ73" s="44">
         <v>19.178000000000001</v>
       </c>
-      <c r="AK73" s="33"/>
-      <c r="AL73" s="33"/>
+      <c r="AK73" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL73" s="45">
+        <v>140.80000000000001</v>
+      </c>
       <c r="AO73" s="8">
         <v>14.2</v>
       </c>
@@ -10817,7 +11120,7 @@
       </c>
     </row>
     <row r="74" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A74" s="42">
+      <c r="A74" s="41">
         <v>73</v>
       </c>
       <c r="B74" s="2" t="s">
@@ -10917,17 +11220,21 @@
       <c r="AG74" s="40">
         <v>0.4289</v>
       </c>
-      <c r="AH74" s="45">
+      <c r="AH74" s="44">
         <v>42.206000000000003</v>
       </c>
-      <c r="AI74" s="45">
+      <c r="AI74" s="44">
         <v>105.15</v>
       </c>
-      <c r="AJ74" s="45">
+      <c r="AJ74" s="44">
         <v>68.328000000000003</v>
       </c>
-      <c r="AK74" s="33"/>
-      <c r="AL74" s="33"/>
+      <c r="AK74" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL74" s="45">
+        <v>99.6</v>
+      </c>
       <c r="AO74" s="8">
         <v>13.6</v>
       </c>
@@ -10942,7 +11249,7 @@
       </c>
     </row>
     <row r="75" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A75" s="42">
+      <c r="A75" s="41">
         <v>74</v>
       </c>
       <c r="B75" s="2" t="s">
@@ -11042,17 +11349,21 @@
       <c r="AG75" s="40">
         <v>0.79259999999999997</v>
       </c>
-      <c r="AH75" s="45">
+      <c r="AH75" s="44">
         <v>116.628</v>
       </c>
-      <c r="AI75" s="45">
+      <c r="AI75" s="44">
         <v>101.791</v>
       </c>
-      <c r="AJ75" s="45">
+      <c r="AJ75" s="44">
         <v>109.104</v>
       </c>
-      <c r="AK75" s="33"/>
-      <c r="AL75" s="33"/>
+      <c r="AK75" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL75" s="45">
+        <v>103.8</v>
+      </c>
       <c r="AO75" s="8">
         <v>14.2</v>
       </c>
@@ -11067,7 +11378,7 @@
       </c>
     </row>
     <row r="76" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A76" s="42">
+      <c r="A76" s="41">
         <v>75</v>
       </c>
       <c r="B76" s="2" t="s">
@@ -11167,17 +11478,21 @@
       <c r="AG76" s="40">
         <v>0.15329999999999999</v>
       </c>
-      <c r="AH76" s="45">
+      <c r="AH76" s="44">
         <v>30.433</v>
       </c>
-      <c r="AI76" s="45">
+      <c r="AI76" s="44">
         <v>30.98</v>
       </c>
-      <c r="AJ76" s="45">
+      <c r="AJ76" s="44">
         <v>28.838000000000001</v>
       </c>
-      <c r="AK76" s="33"/>
-      <c r="AL76" s="33"/>
+      <c r="AK76" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL76" s="45">
+        <v>118.6</v>
+      </c>
       <c r="AO76" s="8">
         <v>17.600000000000001</v>
       </c>
@@ -11192,7 +11507,7 @@
       </c>
     </row>
     <row r="77" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A77" s="42">
+      <c r="A77" s="41">
         <v>76</v>
       </c>
       <c r="B77" s="2" t="s">
@@ -11292,17 +11607,21 @@
       <c r="AG77" s="40">
         <v>0.1072</v>
       </c>
-      <c r="AH77" s="45">
+      <c r="AH77" s="44">
         <v>26.791</v>
       </c>
-      <c r="AI77" s="45">
+      <c r="AI77" s="44">
         <v>20.81</v>
       </c>
-      <c r="AJ77" s="45">
+      <c r="AJ77" s="44">
         <v>21.323</v>
       </c>
-      <c r="AK77" s="33"/>
-      <c r="AL77" s="33"/>
+      <c r="AK77" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL77" s="45">
+        <v>105.2</v>
+      </c>
       <c r="AO77" s="8">
         <v>16.2</v>
       </c>
@@ -11317,7 +11636,7 @@
       </c>
     </row>
     <row r="78" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A78" s="42">
+      <c r="A78" s="41">
         <v>77</v>
       </c>
       <c r="B78" s="2" t="s">
@@ -11417,17 +11736,21 @@
       <c r="AG78" s="40">
         <v>0.33119999999999999</v>
       </c>
-      <c r="AH78" s="45">
+      <c r="AH78" s="44">
         <v>72.888000000000005</v>
       </c>
-      <c r="AI78" s="45">
+      <c r="AI78" s="44">
         <v>111.95</v>
       </c>
-      <c r="AJ78" s="45">
+      <c r="AJ78" s="44">
         <v>60.387</v>
       </c>
-      <c r="AK78" s="33"/>
-      <c r="AL78" s="33"/>
+      <c r="AK78" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL78" s="45">
+        <v>71.8</v>
+      </c>
       <c r="AO78" s="8">
         <v>12</v>
       </c>
@@ -11442,7 +11765,7 @@
       </c>
     </row>
     <row r="79" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A79" s="42">
+      <c r="A79" s="41">
         <v>78</v>
       </c>
       <c r="B79" s="2" t="s">
@@ -11542,17 +11865,21 @@
       <c r="AG79" s="40">
         <v>0.62519999999999998</v>
       </c>
-      <c r="AH79" s="45">
+      <c r="AH79" s="44">
         <v>119.839</v>
       </c>
-      <c r="AI79" s="45">
+      <c r="AI79" s="44">
         <v>133.01900000000001</v>
       </c>
-      <c r="AJ79" s="45">
+      <c r="AJ79" s="44">
         <v>100.142</v>
       </c>
-      <c r="AK79" s="33"/>
-      <c r="AL79" s="33"/>
+      <c r="AK79" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL79" s="45">
+        <v>90</v>
+      </c>
       <c r="AO79" s="8">
         <v>10.9</v>
       </c>
@@ -11567,7 +11894,7 @@
       </c>
     </row>
     <row r="80" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A80" s="42">
+      <c r="A80" s="41">
         <v>79</v>
       </c>
       <c r="B80" s="2" t="s">
@@ -11667,17 +11994,21 @@
       <c r="AG80" s="40">
         <v>9.0800000000000006E-2</v>
       </c>
-      <c r="AH80" s="45">
+      <c r="AH80" s="44">
         <v>29.489000000000001</v>
       </c>
-      <c r="AI80" s="45">
+      <c r="AI80" s="44">
         <v>23.649000000000001</v>
       </c>
-      <c r="AJ80" s="45">
+      <c r="AJ80" s="44">
         <v>22.178000000000001</v>
       </c>
-      <c r="AK80" s="33"/>
-      <c r="AL80" s="33"/>
+      <c r="AK80" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL80" s="45">
+        <v>96.2</v>
+      </c>
       <c r="AO80" s="8">
         <v>16</v>
       </c>
@@ -11692,7 +12023,7 @@
       </c>
     </row>
     <row r="81" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A81" s="42">
+      <c r="A81" s="41">
         <v>80</v>
       </c>
       <c r="B81" s="2" t="s">
@@ -11792,17 +12123,21 @@
       <c r="AG81" s="40">
         <v>0.13239999999999999</v>
       </c>
-      <c r="AH81" s="45">
+      <c r="AH81" s="44">
         <v>30.081</v>
       </c>
-      <c r="AI81" s="45">
+      <c r="AI81" s="44">
         <v>27.806000000000001</v>
       </c>
-      <c r="AJ81" s="45">
+      <c r="AJ81" s="44">
         <v>26.933</v>
       </c>
-      <c r="AK81" s="33"/>
-      <c r="AL81" s="33"/>
+      <c r="AK81" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL81" s="45">
+        <v>83.6</v>
+      </c>
       <c r="AO81" s="8">
         <v>13.3</v>
       </c>
@@ -11817,7 +12152,7 @@
       </c>
     </row>
     <row r="82" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A82" s="42">
+      <c r="A82" s="41">
         <v>81</v>
       </c>
       <c r="B82" s="2" t="s">
@@ -11917,14 +12252,20 @@
       <c r="AG82" s="40">
         <v>1.4646999999999999</v>
       </c>
-      <c r="AH82" s="45">
+      <c r="AH82" s="44">
         <v>183.59100000000001</v>
       </c>
-      <c r="AI82" s="45">
+      <c r="AI82" s="44">
         <v>170.37899999999999</v>
       </c>
-      <c r="AJ82" s="45">
+      <c r="AJ82" s="44">
         <v>196.001</v>
+      </c>
+      <c r="AK82" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL82" s="44">
+        <v>112.4</v>
       </c>
       <c r="AO82" s="8">
         <v>13.8</v>
@@ -11940,7 +12281,7 @@
       </c>
     </row>
     <row r="83" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A83" s="42">
+      <c r="A83" s="41">
         <v>82</v>
       </c>
       <c r="B83" s="2" t="s">
@@ -12040,14 +12381,20 @@
       <c r="AG83" s="40">
         <v>0.14580000000000001</v>
       </c>
-      <c r="AH83" s="45">
+      <c r="AH83" s="44">
         <v>36.978000000000002</v>
       </c>
-      <c r="AI83" s="45">
+      <c r="AI83" s="44">
         <v>30.055</v>
       </c>
-      <c r="AJ83" s="45">
+      <c r="AJ83" s="44">
         <v>25.213999999999999</v>
+      </c>
+      <c r="AK83" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL83" s="44">
+        <v>128.4</v>
       </c>
       <c r="AO83" s="8">
         <v>19.7</v>
@@ -12063,7 +12410,7 @@
       </c>
     </row>
     <row r="84" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A84" s="42">
+      <c r="A84" s="41">
         <v>83</v>
       </c>
       <c r="B84" s="2" t="s">
@@ -12163,14 +12510,20 @@
       <c r="AG84" s="40">
         <v>0.75880000000000003</v>
       </c>
-      <c r="AH84" s="45">
+      <c r="AH84" s="44">
         <v>93.085999999999999</v>
       </c>
-      <c r="AI84" s="45">
+      <c r="AI84" s="44">
         <v>106.337</v>
       </c>
-      <c r="AJ84" s="45">
+      <c r="AJ84" s="44">
         <v>140.279</v>
+      </c>
+      <c r="AK84" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL84" s="44">
+        <v>107.4</v>
       </c>
       <c r="AO84" s="8">
         <v>10.9</v>
@@ -12186,7 +12539,7 @@
       </c>
     </row>
     <row r="85" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A85" s="42">
+      <c r="A85" s="41">
         <v>84</v>
       </c>
       <c r="B85" s="2" t="s">
@@ -12286,14 +12639,20 @@
       <c r="AG85" s="40">
         <v>0.161</v>
       </c>
-      <c r="AH85" s="45">
+      <c r="AH85" s="44">
         <v>35.716000000000001</v>
       </c>
-      <c r="AI85" s="45">
+      <c r="AI85" s="44">
         <v>38.152000000000001</v>
       </c>
-      <c r="AJ85" s="45">
+      <c r="AJ85" s="44">
         <v>31.721</v>
+      </c>
+      <c r="AK85" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL85" s="44">
+        <v>92.6</v>
       </c>
       <c r="AO85" s="8">
         <v>13.3</v>
@@ -12309,7 +12668,7 @@
       </c>
     </row>
     <row r="86" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A86" s="42">
+      <c r="A86" s="41">
         <v>85</v>
       </c>
       <c r="B86" s="2" t="s">
@@ -12409,14 +12768,20 @@
       <c r="AG86" s="40">
         <v>0.97470000000000001</v>
       </c>
-      <c r="AH86" s="45">
+      <c r="AH86" s="44">
         <v>114.95</v>
       </c>
-      <c r="AI86" s="45">
+      <c r="AI86" s="44">
         <v>62.869</v>
       </c>
-      <c r="AJ86" s="45">
+      <c r="AJ86" s="44">
         <v>164.881</v>
+      </c>
+      <c r="AK86" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL86" s="44">
+        <v>104.6</v>
       </c>
       <c r="AO86" s="8">
         <v>12</v>
@@ -12432,7 +12797,7 @@
       </c>
     </row>
     <row r="87" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A87" s="42">
+      <c r="A87" s="41">
         <v>86</v>
       </c>
       <c r="B87" s="2" t="s">
@@ -12532,17 +12897,21 @@
       <c r="AG87" s="40">
         <v>0.1908</v>
       </c>
-      <c r="AH87" s="45">
+      <c r="AH87" s="44">
         <v>50.915999999999997</v>
       </c>
-      <c r="AI87" s="45">
+      <c r="AI87" s="44">
         <v>46.648000000000003</v>
       </c>
-      <c r="AJ87" s="45">
+      <c r="AJ87" s="44">
         <v>37.262999999999998</v>
       </c>
-      <c r="AK87" s="33"/>
-      <c r="AL87" s="33"/>
+      <c r="AK87" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL87" s="45">
+        <v>105.2</v>
+      </c>
       <c r="AO87" s="8">
         <v>17.399999999999999</v>
       </c>
@@ -12557,7 +12926,7 @@
       </c>
     </row>
     <row r="88" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A88" s="42">
+      <c r="A88" s="41">
         <v>87</v>
       </c>
       <c r="B88" s="2" t="s">
@@ -12657,17 +13026,21 @@
       <c r="AG88" s="40">
         <v>0.34389999999999998</v>
       </c>
-      <c r="AH88" s="45">
+      <c r="AH88" s="44">
         <v>117.15</v>
       </c>
-      <c r="AI88" s="45">
+      <c r="AI88" s="44">
         <v>111.22499999999999</v>
       </c>
-      <c r="AJ88" s="45">
+      <c r="AJ88" s="44">
         <v>62.850999999999999</v>
       </c>
-      <c r="AK88" s="33"/>
-      <c r="AL88" s="33"/>
+      <c r="AK88" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL88" s="45">
+        <v>114.8</v>
+      </c>
       <c r="AO88" s="8">
         <v>14.8</v>
       </c>
@@ -12682,7 +13055,7 @@
       </c>
     </row>
     <row r="89" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A89" s="42">
+      <c r="A89" s="41">
         <v>88</v>
       </c>
       <c r="B89" s="2" t="s">
@@ -12782,17 +13155,21 @@
       <c r="AG89" s="40">
         <v>0.1946</v>
       </c>
-      <c r="AH89" s="45">
+      <c r="AH89" s="44">
         <v>41.03</v>
       </c>
-      <c r="AI89" s="45">
+      <c r="AI89" s="44">
         <v>40.127000000000002</v>
       </c>
-      <c r="AJ89" s="45">
+      <c r="AJ89" s="44">
         <v>37.5</v>
       </c>
-      <c r="AK89" s="33"/>
-      <c r="AL89" s="33"/>
+      <c r="AK89" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL89" s="45">
+        <v>134.4</v>
+      </c>
       <c r="AO89" s="8">
         <v>18.399999999999999</v>
       </c>
@@ -12807,7 +13184,7 @@
       </c>
     </row>
     <row r="90" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A90" s="42">
+      <c r="A90" s="41">
         <v>89</v>
       </c>
       <c r="B90" s="2" t="s">
@@ -12907,17 +13284,21 @@
       <c r="AG90" s="40">
         <v>0.40949999999999998</v>
       </c>
-      <c r="AH90" s="45">
+      <c r="AH90" s="44">
         <v>97.192999999999998</v>
       </c>
-      <c r="AI90" s="45">
+      <c r="AI90" s="44">
         <v>108.91800000000001</v>
       </c>
-      <c r="AJ90" s="45">
+      <c r="AJ90" s="44">
         <v>66.582999999999998</v>
       </c>
-      <c r="AK90" s="33"/>
-      <c r="AL90" s="33"/>
+      <c r="AK90" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL90" s="45">
+        <v>158.80000000000001</v>
+      </c>
       <c r="AO90" s="8">
         <v>15.6</v>
       </c>
@@ -12932,7 +13313,7 @@
       </c>
     </row>
     <row r="91" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A91" s="42">
+      <c r="A91" s="41">
         <v>90</v>
       </c>
       <c r="B91" s="2" t="s">
@@ -13032,17 +13413,21 @@
       <c r="AG91" s="40">
         <v>0.13850000000000001</v>
       </c>
-      <c r="AH91" s="45">
+      <c r="AH91" s="44">
         <v>28.664999999999999</v>
       </c>
-      <c r="AI91" s="45">
+      <c r="AI91" s="44">
         <v>28.574000000000002</v>
       </c>
-      <c r="AJ91" s="45">
+      <c r="AJ91" s="44">
         <v>26.210999999999999</v>
       </c>
-      <c r="AK91" s="33"/>
-      <c r="AL91" s="33"/>
+      <c r="AK91" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL91" s="45">
+        <v>114.2</v>
+      </c>
       <c r="AO91" s="8">
         <v>19</v>
       </c>
@@ -13057,7 +13442,7 @@
       </c>
     </row>
     <row r="92" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A92" s="42">
+      <c r="A92" s="41">
         <v>91</v>
       </c>
       <c r="B92" s="2" t="s">
@@ -13157,17 +13542,21 @@
       <c r="AG92" s="40">
         <v>0.55289999999999995</v>
       </c>
-      <c r="AH92" s="45">
+      <c r="AH92" s="44">
         <v>107.306</v>
       </c>
-      <c r="AI92" s="45">
+      <c r="AI92" s="44">
         <v>110.02800000000001</v>
       </c>
-      <c r="AJ92" s="45">
+      <c r="AJ92" s="44">
         <v>98.87</v>
       </c>
-      <c r="AK92" s="33"/>
-      <c r="AL92" s="33"/>
+      <c r="AK92" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL92" s="45">
+        <v>54.6</v>
+      </c>
       <c r="AO92" s="8">
         <v>8.6999999999999993</v>
       </c>
@@ -13182,7 +13571,7 @@
       </c>
     </row>
     <row r="93" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A93" s="42">
+      <c r="A93" s="41">
         <v>92</v>
       </c>
       <c r="B93" s="2" t="s">
@@ -13282,14 +13671,20 @@
       <c r="AG93" s="40">
         <v>9.11E-2</v>
       </c>
-      <c r="AH93" s="45">
+      <c r="AH93" s="44">
         <v>19.257999999999999</v>
       </c>
-      <c r="AI93" s="45">
+      <c r="AI93" s="44">
         <v>20.225000000000001</v>
       </c>
-      <c r="AJ93" s="45">
+      <c r="AJ93" s="44">
         <v>17.728999999999999</v>
+      </c>
+      <c r="AK93" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL93" s="44">
+        <v>67.2</v>
       </c>
       <c r="AO93" s="8">
         <v>13.3</v>
@@ -13303,7 +13698,7 @@
       </c>
     </row>
     <row r="94" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A94" s="42">
+      <c r="A94" s="41">
         <v>93</v>
       </c>
       <c r="B94" s="2" t="s">
@@ -13403,17 +13798,21 @@
       <c r="AG94" s="40">
         <v>0.57940000000000003</v>
       </c>
-      <c r="AH94" s="45">
+      <c r="AH94" s="44">
         <v>75.543999999999997</v>
       </c>
-      <c r="AI94" s="45">
+      <c r="AI94" s="44">
         <v>52.244</v>
       </c>
-      <c r="AJ94" s="45">
+      <c r="AJ94" s="44">
         <v>79.573999999999998</v>
       </c>
-      <c r="AK94" s="33"/>
-      <c r="AL94" s="33"/>
+      <c r="AK94" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL94" s="45">
+        <v>178.8</v>
+      </c>
       <c r="AO94" s="8">
         <v>15.7</v>
       </c>
@@ -13428,7 +13827,7 @@
       </c>
     </row>
     <row r="95" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A95" s="42">
+      <c r="A95" s="41">
         <v>94</v>
       </c>
       <c r="B95" s="2" t="s">
@@ -13528,17 +13927,21 @@
       <c r="AG95" s="40">
         <v>0.1419</v>
       </c>
-      <c r="AH95" s="45">
+      <c r="AH95" s="44">
         <v>39.186999999999998</v>
       </c>
-      <c r="AI95" s="45">
+      <c r="AI95" s="44">
         <v>36.814</v>
       </c>
-      <c r="AJ95" s="45">
+      <c r="AJ95" s="44">
         <v>28.465</v>
       </c>
-      <c r="AK95" s="33"/>
-      <c r="AL95" s="33"/>
+      <c r="AK95" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL95" s="45">
+        <v>176.6</v>
+      </c>
       <c r="AO95" s="8">
         <v>21.8</v>
       </c>
@@ -13553,7 +13956,7 @@
       </c>
     </row>
     <row r="96" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A96" s="42">
+      <c r="A96" s="41">
         <v>95</v>
       </c>
       <c r="B96" s="2" t="s">
@@ -13653,17 +14056,21 @@
       <c r="AG96" s="40">
         <v>0.4677</v>
       </c>
-      <c r="AH96" s="45">
+      <c r="AH96" s="44">
         <v>82.489000000000004</v>
       </c>
-      <c r="AI96" s="45">
+      <c r="AI96" s="44">
         <v>73.766999999999996</v>
       </c>
-      <c r="AJ96" s="45">
+      <c r="AJ96" s="44">
         <v>67.700999999999993</v>
       </c>
-      <c r="AK96" s="33"/>
-      <c r="AL96" s="33"/>
+      <c r="AK96" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL96" s="45">
+        <v>133.19999999999999</v>
+      </c>
       <c r="AO96" s="8">
         <v>15</v>
       </c>
@@ -13678,7 +14085,7 @@
       </c>
     </row>
     <row r="97" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A97" s="42">
+      <c r="A97" s="41">
         <v>96</v>
       </c>
       <c r="B97" s="2" t="s">
@@ -13778,17 +14185,21 @@
       <c r="AG97" s="40">
         <v>0.1426</v>
       </c>
-      <c r="AH97" s="45">
+      <c r="AH97" s="44">
         <v>34.716999999999999</v>
       </c>
-      <c r="AI97" s="45">
+      <c r="AI97" s="44">
         <v>30.074000000000002</v>
       </c>
-      <c r="AJ97" s="45">
+      <c r="AJ97" s="44">
         <v>27.792000000000002</v>
       </c>
-      <c r="AK97" s="33"/>
-      <c r="AL97" s="33"/>
+      <c r="AK97" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL97" s="45">
+        <v>99.6</v>
+      </c>
       <c r="AO97" s="8">
         <v>15.4</v>
       </c>
@@ -13803,7 +14214,7 @@
       </c>
     </row>
     <row r="98" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A98" s="42">
+      <c r="A98" s="41">
         <v>97</v>
       </c>
       <c r="B98" s="2" t="s">
@@ -13903,14 +14314,20 @@
       <c r="AG98" s="40">
         <v>0.4662</v>
       </c>
-      <c r="AH98" s="45">
+      <c r="AH98" s="44">
         <v>76.685000000000002</v>
       </c>
-      <c r="AI98" s="45">
+      <c r="AI98" s="44">
         <v>74.566000000000003</v>
       </c>
-      <c r="AJ98" s="45">
+      <c r="AJ98" s="44">
         <v>76.192999999999998</v>
+      </c>
+      <c r="AK98" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL98" s="44">
+        <v>136</v>
       </c>
       <c r="AO98" s="8">
         <v>14.5</v>
@@ -13926,7 +14343,7 @@
       </c>
     </row>
     <row r="99" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A99" s="42">
+      <c r="A99" s="41">
         <v>98</v>
       </c>
       <c r="B99" s="2" t="s">
@@ -14026,17 +14443,21 @@
       <c r="AG99" s="40">
         <v>0.14330000000000001</v>
       </c>
-      <c r="AH99" s="45">
+      <c r="AH99" s="44">
         <v>41.094999999999999</v>
       </c>
-      <c r="AI99" s="45">
+      <c r="AI99" s="44">
         <v>37.786999999999999</v>
       </c>
-      <c r="AJ99" s="45">
+      <c r="AJ99" s="44">
         <v>27.815999999999999</v>
       </c>
-      <c r="AK99" s="33"/>
-      <c r="AL99" s="33"/>
+      <c r="AK99" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL99" s="45">
+        <v>110</v>
+      </c>
       <c r="AO99" s="8">
         <v>17.8</v>
       </c>
@@ -14051,7 +14472,7 @@
       </c>
     </row>
     <row r="100" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A100" s="42">
+      <c r="A100" s="41">
         <v>99</v>
       </c>
       <c r="B100" s="2" t="s">
@@ -14151,17 +14572,21 @@
       <c r="AG100" s="40">
         <v>0.50849999999999995</v>
       </c>
-      <c r="AH100" s="45">
+      <c r="AH100" s="44">
         <v>73.387</v>
       </c>
-      <c r="AI100" s="45">
+      <c r="AI100" s="44">
         <v>85.064999999999998</v>
       </c>
-      <c r="AJ100" s="45">
+      <c r="AJ100" s="44">
         <v>78.802000000000007</v>
       </c>
-      <c r="AK100" s="33"/>
-      <c r="AL100" s="33"/>
+      <c r="AK100" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL100" s="45">
+        <v>186.4</v>
+      </c>
       <c r="AO100" s="2">
         <v>21.7</v>
       </c>
@@ -14176,7 +14601,7 @@
       </c>
     </row>
     <row r="101" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A101" s="42">
+      <c r="A101" s="41">
         <v>100</v>
       </c>
       <c r="B101" s="2" t="s">
@@ -14276,17 +14701,21 @@
       <c r="AG101" s="40">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="AH101" s="45">
+      <c r="AH101" s="44">
         <v>22.992999999999999</v>
       </c>
-      <c r="AI101" s="45">
+      <c r="AI101" s="44">
         <v>19.559999999999999</v>
       </c>
-      <c r="AJ101" s="45">
+      <c r="AJ101" s="44">
         <v>16.484000000000002</v>
       </c>
-      <c r="AK101" s="33"/>
-      <c r="AL101" s="33"/>
+      <c r="AK101" s="45">
+        <v>22</v>
+      </c>
+      <c r="AL101" s="45">
+        <v>75.8</v>
+      </c>
       <c r="AO101" s="2">
         <v>21.6</v>
       </c>
@@ -16696,13 +17125,13 @@
       <c r="A2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="46" t="s">
         <v>143</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
       <c r="H2" t="s">
         <v>118</v>
       </c>
@@ -17136,13 +17565,13 @@
       <c r="A27" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="41" t="s">
+      <c r="B27" s="46" t="s">
         <v>149</v>
       </c>
-      <c r="C27" s="41"/>
-      <c r="D27" s="41"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="41"/>
+      <c r="C27" s="46"/>
+      <c r="D27" s="46"/>
+      <c r="E27" s="46"/>
+      <c r="F27" s="46"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -17533,13 +17962,13 @@
       <c r="A52" t="s">
         <v>10</v>
       </c>
-      <c r="B52" s="41" t="s">
+      <c r="B52" s="46" t="s">
         <v>150</v>
       </c>
-      <c r="C52" s="41"/>
-      <c r="D52" s="41"/>
-      <c r="E52" s="41"/>
-      <c r="F52" s="41"/>
+      <c r="C52" s="46"/>
+      <c r="D52" s="46"/>
+      <c r="E52" s="46"/>
+      <c r="F52" s="46"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">

</xml_diff>

<commit_message>
Adjust form of r scripts
</commit_message>
<xml_diff>
--- a/data/raw/data_raw.xlsx
+++ b/data/raw/data_raw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Documents\0_Ziegelprojekt\3_Aufnahmen_und_Ergebnisse\2020_waste_bricks_trees\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA79F8B-2BFA-400C-9711-A5D0BA019728}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED470ECD-1BCA-4EC2-B2D9-03241673F0CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20055" yWindow="990" windowWidth="8745" windowHeight="16305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data raw" sheetId="1" r:id="rId1"/>
@@ -118,7 +118,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R64" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
+    <comment ref="R65" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -144,7 +144,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R80" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
+    <comment ref="R81" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
           <rPr>
@@ -170,7 +170,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R82" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
+    <comment ref="R83" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
       <text>
         <r>
           <rPr>
@@ -196,7 +196,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R89" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
+    <comment ref="R90" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
       <text>
         <r>
           <rPr>
@@ -418,7 +418,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1437" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1443" uniqueCount="271">
   <si>
     <t>brickRatio</t>
   </si>
@@ -1222,6 +1222,15 @@
   </si>
   <si>
     <t>rootorder</t>
+  </si>
+  <si>
+    <t>rootVolume</t>
+  </si>
+  <si>
+    <t>cm^3</t>
+  </si>
+  <si>
+    <t>Volume of roots of fine root sample of category I to III</t>
   </si>
 </sst>
 </file>
@@ -1713,11 +1722,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AW126"/>
+  <dimension ref="A1:AX126"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="AC1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AM21" sqref="AM21"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1752,16 +1761,17 @@
     <col min="36" max="36" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="10.7109375" style="46" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="27" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="10.7109375" customWidth="1"/>
-    <col min="49" max="16384" width="11.42578125" style="2"/>
+    <col min="39" max="39" width="11.7109375" style="27" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="26" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="18.85546875" customWidth="1"/>
+    <col min="45" max="45" width="10.7109375" customWidth="1"/>
+    <col min="50" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:45" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>113</v>
       </c>
@@ -1877,25 +1887,28 @@
         <v>228</v>
       </c>
       <c r="AM1" s="29" t="s">
+        <v>268</v>
+      </c>
+      <c r="AN1" s="29" t="s">
         <v>255</v>
       </c>
-      <c r="AN1" s="29" t="s">
+      <c r="AO1" s="29" t="s">
         <v>248</v>
       </c>
-      <c r="AO1" s="29" t="s">
+      <c r="AP1" s="29" t="s">
         <v>256</v>
       </c>
-      <c r="AP1" s="29" t="s">
+      <c r="AQ1" s="29" t="s">
         <v>249</v>
       </c>
-      <c r="AQ1" s="29" t="s">
+      <c r="AR1" s="29" t="s">
         <v>261</v>
       </c>
-      <c r="AR1" s="29" t="s">
+      <c r="AS1" s="29" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A2" s="40">
         <v>1</v>
       </c>
@@ -2010,26 +2023,29 @@
       <c r="AL2" s="46">
         <v>497.39490000000001</v>
       </c>
-      <c r="AM2" s="45">
+      <c r="AM2" s="27">
+        <v>0.47399999999999998</v>
+      </c>
+      <c r="AN2" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN2" s="49">
+      <c r="AO2" s="49">
         <v>3.6</v>
       </c>
-      <c r="AO2" s="45">
+      <c r="AP2" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP2" s="49">
+      <c r="AQ2" s="49">
         <v>3.5329999999999999</v>
       </c>
-      <c r="AQ2" s="42" t="s">
+      <c r="AR2" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="AR2" s="46">
+      <c r="AS2" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A3" s="40">
         <v>2</v>
       </c>
@@ -2144,26 +2160,29 @@
       <c r="AL3" s="46">
         <v>1465.5363</v>
       </c>
-      <c r="AM3" s="45">
+      <c r="AM3" s="27">
+        <v>1.3109999999999999</v>
+      </c>
+      <c r="AN3" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN3" s="49">
+      <c r="AO3" s="49">
         <v>3.774</v>
       </c>
-      <c r="AO3" s="45">
+      <c r="AP3" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP3" s="49">
+      <c r="AQ3" s="49">
         <v>4.0739999999999998</v>
       </c>
-      <c r="AQ3" s="42" t="s">
+      <c r="AR3" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="AR3" s="46">
+      <c r="AS3" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A4" s="40">
         <v>3</v>
       </c>
@@ -2278,26 +2297,29 @@
       <c r="AL4" s="46">
         <v>735.74800000000005</v>
       </c>
-      <c r="AM4" s="45">
+      <c r="AM4" s="27">
+        <v>0.37</v>
+      </c>
+      <c r="AN4" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN4" s="49">
+      <c r="AO4" s="49">
         <v>3.5369999999999999</v>
       </c>
-      <c r="AO4" s="45">
+      <c r="AP4" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP4" s="50">
+      <c r="AQ4" s="50">
         <v>3.7160000000000002</v>
       </c>
-      <c r="AQ4" s="42" t="s">
+      <c r="AR4" s="42" t="s">
         <v>262</v>
       </c>
-      <c r="AR4" s="46">
+      <c r="AS4" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A5" s="40">
         <v>4</v>
       </c>
@@ -2412,26 +2434,29 @@
       <c r="AL5" s="46">
         <v>844.89</v>
       </c>
-      <c r="AM5" s="45">
+      <c r="AM5" s="27">
+        <v>0.39200000000000002</v>
+      </c>
+      <c r="AN5" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN5" s="49">
+      <c r="AO5" s="49">
         <v>3.4910000000000001</v>
       </c>
-      <c r="AO5" s="45">
+      <c r="AP5" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP5" s="50">
+      <c r="AQ5" s="50">
         <v>3.5939999999999999</v>
       </c>
-      <c r="AQ5" s="42" t="s">
+      <c r="AR5" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="AR5" s="46">
+      <c r="AS5" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A6" s="40">
         <v>5</v>
       </c>
@@ -2546,26 +2571,29 @@
       <c r="AL6" s="46">
         <v>1634.277</v>
       </c>
-      <c r="AM6" s="45">
+      <c r="AM6" s="27">
+        <v>1.157</v>
+      </c>
+      <c r="AN6" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN6" s="49">
+      <c r="AO6" s="49">
         <v>3.7090000000000001</v>
       </c>
-      <c r="AO6" s="45">
+      <c r="AP6" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP6" s="50">
+      <c r="AQ6" s="50">
         <v>3.74</v>
       </c>
-      <c r="AQ6" s="42" t="s">
+      <c r="AR6" s="42" t="s">
         <v>262</v>
       </c>
-      <c r="AR6" s="46">
+      <c r="AS6" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A7" s="40">
         <v>6</v>
       </c>
@@ -2680,26 +2708,29 @@
       <c r="AL7" s="46">
         <v>1027.3219999999999</v>
       </c>
-      <c r="AM7" s="45">
+      <c r="AM7" s="27">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="AN7" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN7" s="49">
+      <c r="AO7" s="49">
         <v>3.7909999999999999</v>
       </c>
-      <c r="AO7" s="45">
+      <c r="AP7" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP7" s="50">
+      <c r="AQ7" s="50">
         <v>3.669</v>
       </c>
-      <c r="AQ7" s="42" t="s">
+      <c r="AR7" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="AR7" s="46">
+      <c r="AS7" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A8" s="40">
         <v>7</v>
       </c>
@@ -2814,26 +2845,29 @@
       <c r="AL8" s="46">
         <v>1353.6220000000001</v>
       </c>
-      <c r="AM8" s="45">
+      <c r="AM8" s="27">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="AN8" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN8" s="49">
+      <c r="AO8" s="49">
         <v>3.7589999999999999</v>
       </c>
-      <c r="AO8" s="45">
+      <c r="AP8" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP8" s="50">
+      <c r="AQ8" s="50">
         <v>3.694</v>
       </c>
-      <c r="AQ8" s="42" t="s">
+      <c r="AR8" s="42" t="s">
         <v>262</v>
       </c>
-      <c r="AR8" s="46">
+      <c r="AS8" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A9" s="40">
         <v>8</v>
       </c>
@@ -2948,26 +2982,29 @@
       <c r="AL9" s="46">
         <v>1771.5319999999999</v>
       </c>
-      <c r="AM9" s="45">
+      <c r="AM9" s="27">
+        <v>1.073</v>
+      </c>
+      <c r="AN9" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN9" s="49">
+      <c r="AO9" s="49">
         <v>3.8690000000000002</v>
       </c>
-      <c r="AO9" s="45">
+      <c r="AP9" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP9" s="50">
+      <c r="AQ9" s="50">
         <v>4.1050000000000004</v>
       </c>
-      <c r="AQ9" s="42" t="s">
+      <c r="AR9" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="AR9" s="46">
+      <c r="AS9" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A10" s="40">
         <v>9</v>
       </c>
@@ -3082,26 +3119,29 @@
       <c r="AL10" s="46">
         <v>1213.856</v>
       </c>
-      <c r="AM10" s="45">
+      <c r="AM10" s="27">
+        <v>1.46</v>
+      </c>
+      <c r="AN10" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN10" s="49">
+      <c r="AO10" s="49">
         <v>3.742</v>
       </c>
-      <c r="AO10" s="45">
+      <c r="AP10" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP10" s="50">
+      <c r="AQ10" s="50">
         <v>3.6349999999999998</v>
       </c>
-      <c r="AQ10" s="42" t="s">
+      <c r="AR10" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="AR10" s="46">
+      <c r="AS10" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A11" s="40">
         <v>10</v>
       </c>
@@ -3216,26 +3256,29 @@
       <c r="AL11" s="46">
         <v>1560.816</v>
       </c>
-      <c r="AM11" s="45">
+      <c r="AM11" s="27">
+        <v>1.026</v>
+      </c>
+      <c r="AN11" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN11" s="49">
+      <c r="AO11" s="49">
         <v>3.742</v>
       </c>
-      <c r="AO11" s="45">
+      <c r="AP11" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP11" s="50">
+      <c r="AQ11" s="50">
         <v>3.613</v>
       </c>
-      <c r="AQ11" s="42" t="s">
+      <c r="AR11" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="AR11" s="46">
+      <c r="AS11" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A12" s="40">
         <v>11</v>
       </c>
@@ -3350,26 +3393,29 @@
       <c r="AL12" s="46">
         <v>235.42699999999999</v>
       </c>
-      <c r="AM12" s="45">
+      <c r="AM12" s="27">
+        <v>0.185</v>
+      </c>
+      <c r="AN12" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN12" s="49">
+      <c r="AO12" s="49">
         <v>3.4209999999999998</v>
       </c>
-      <c r="AO12" s="45">
+      <c r="AP12" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP12" s="49">
+      <c r="AQ12" s="49">
         <v>3.5569999999999999</v>
       </c>
-      <c r="AQ12" s="42" t="s">
+      <c r="AR12" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="AR12" s="46">
+      <c r="AS12" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A13" s="40">
         <v>12</v>
       </c>
@@ -3484,26 +3530,29 @@
       <c r="AL13" s="46">
         <v>775.82</v>
       </c>
-      <c r="AM13" s="45">
+      <c r="AM13" s="27">
+        <v>0.37</v>
+      </c>
+      <c r="AN13" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN13" s="49">
+      <c r="AO13" s="49">
         <v>3.508</v>
       </c>
-      <c r="AO13" s="45">
+      <c r="AP13" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP13" s="49">
+      <c r="AQ13" s="49">
         <v>3.657</v>
       </c>
-      <c r="AQ13" s="42" t="s">
+      <c r="AR13" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="AR13" s="46">
+      <c r="AS13" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A14" s="40">
         <v>13</v>
       </c>
@@ -3618,26 +3667,29 @@
       <c r="AL14" s="46">
         <v>448.34399999999999</v>
       </c>
-      <c r="AM14" s="45">
+      <c r="AM14" s="27">
+        <v>0.39700000000000002</v>
+      </c>
+      <c r="AN14" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN14" s="49">
+      <c r="AO14" s="49">
         <v>3.53</v>
       </c>
-      <c r="AO14" s="45">
+      <c r="AP14" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP14" s="49">
+      <c r="AQ14" s="49">
         <v>3.6070000000000002</v>
       </c>
-      <c r="AQ14" s="42" t="s">
+      <c r="AR14" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="AR14" s="46">
+      <c r="AS14" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A15" s="40">
         <v>14</v>
       </c>
@@ -3752,26 +3804,29 @@
       <c r="AL15" s="46">
         <v>673.42399999999998</v>
       </c>
-      <c r="AM15" s="45">
+      <c r="AM15" s="27">
+        <v>0.61099999999999999</v>
+      </c>
+      <c r="AN15" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN15" s="49">
+      <c r="AO15" s="49">
         <v>3.6190000000000002</v>
       </c>
-      <c r="AO15" s="45">
+      <c r="AP15" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP15" s="49">
+      <c r="AQ15" s="49">
         <v>3.6760000000000002</v>
       </c>
-      <c r="AQ15" s="42" t="s">
+      <c r="AR15" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="AR15" s="46">
+      <c r="AS15" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A16" s="40">
         <v>15</v>
       </c>
@@ -3886,26 +3941,29 @@
       <c r="AL16" s="46">
         <v>451.96800000000002</v>
       </c>
-      <c r="AM16" s="45">
+      <c r="AM16" s="27">
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="AN16" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN16" s="49">
+      <c r="AO16" s="49">
         <v>3.4969999999999999</v>
       </c>
-      <c r="AO16" s="45">
+      <c r="AP16" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP16" s="49">
+      <c r="AQ16" s="49">
         <v>3.492</v>
       </c>
-      <c r="AQ16" s="42" t="s">
+      <c r="AR16" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="AR16" s="46">
+      <c r="AS16" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A17" s="40">
         <v>16</v>
       </c>
@@ -4020,26 +4078,29 @@
       <c r="AL17" s="46">
         <v>1282.652</v>
       </c>
-      <c r="AM17" s="45">
+      <c r="AM17" s="27">
+        <v>0.80300000000000005</v>
+      </c>
+      <c r="AN17" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN17" s="49">
+      <c r="AO17" s="49">
         <v>3.6840000000000002</v>
       </c>
-      <c r="AO17" s="45">
+      <c r="AP17" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP17" s="49">
+      <c r="AQ17" s="49">
         <v>3.73</v>
       </c>
-      <c r="AQ17" s="42" t="s">
+      <c r="AR17" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="AR17" s="46">
+      <c r="AS17" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A18" s="40">
         <v>17</v>
       </c>
@@ -4154,26 +4215,29 @@
       <c r="AL18" s="46">
         <v>1107.019</v>
       </c>
-      <c r="AM18" s="45">
+      <c r="AM18" s="27">
+        <v>1.1830000000000001</v>
+      </c>
+      <c r="AN18" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN18" s="49">
+      <c r="AO18" s="49">
         <v>3.782</v>
       </c>
-      <c r="AO18" s="45">
+      <c r="AP18" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP18" s="49">
+      <c r="AQ18" s="49">
         <v>3.5870000000000002</v>
       </c>
-      <c r="AQ18" s="42" t="s">
+      <c r="AR18" s="42" t="s">
         <v>264</v>
       </c>
-      <c r="AR18" s="46">
+      <c r="AS18" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A19" s="40">
         <v>18</v>
       </c>
@@ -4288,26 +4352,29 @@
       <c r="AL19" s="46">
         <v>890.63</v>
       </c>
-      <c r="AM19" s="45">
+      <c r="AM19" s="27">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="AN19" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN19" s="49">
+      <c r="AO19" s="49">
         <v>3.6190000000000002</v>
       </c>
-      <c r="AO19" s="45">
+      <c r="AP19" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP19" s="49">
+      <c r="AQ19" s="49">
         <v>3.6179999999999999</v>
       </c>
-      <c r="AQ19" s="42" t="s">
+      <c r="AR19" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="AR19" s="46">
+      <c r="AS19" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A20" s="40">
         <v>19</v>
       </c>
@@ -4422,26 +4489,29 @@
       <c r="AL20" s="46">
         <v>709.22900000000004</v>
       </c>
-      <c r="AM20" s="45">
+      <c r="AM20" s="27">
+        <v>0.39800000000000002</v>
+      </c>
+      <c r="AN20" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN20" s="49">
+      <c r="AO20" s="49">
         <v>3.5680000000000001</v>
       </c>
-      <c r="AO20" s="45">
+      <c r="AP20" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP20" s="49">
+      <c r="AQ20" s="49">
         <v>4.2560000000000002</v>
       </c>
-      <c r="AQ20" s="42" t="s">
+      <c r="AR20" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="AR20" s="46">
+      <c r="AS20" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A21" s="40">
         <v>20</v>
       </c>
@@ -4556,26 +4626,29 @@
       <c r="AL21" s="46">
         <v>1064.5519999999999</v>
       </c>
-      <c r="AM21" s="45">
+      <c r="AM21" s="27">
+        <v>2.0950000000000002</v>
+      </c>
+      <c r="AN21" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN21" s="49">
+      <c r="AO21" s="49">
         <v>3.6520000000000001</v>
       </c>
-      <c r="AO21" s="45">
+      <c r="AP21" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP21" s="49">
+      <c r="AQ21" s="49">
         <v>4.0270000000000001</v>
       </c>
-      <c r="AQ21" t="s">
+      <c r="AR21" t="s">
         <v>264</v>
       </c>
-      <c r="AR21" s="46">
+      <c r="AS21" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="22" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A22" s="40">
         <v>21</v>
       </c>
@@ -4690,26 +4763,29 @@
       <c r="AL22" s="46">
         <v>608.93200000000002</v>
       </c>
-      <c r="AM22" s="45">
+      <c r="AM22" s="27">
+        <v>0.46300000000000002</v>
+      </c>
+      <c r="AN22" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN22" s="50">
+      <c r="AO22" s="50">
         <v>3.5649999999999999</v>
       </c>
-      <c r="AO22" s="45">
+      <c r="AP22" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP22" s="50">
+      <c r="AQ22" s="50">
         <v>3.496</v>
       </c>
-      <c r="AQ22" s="42" t="s">
+      <c r="AR22" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="AR22" s="46">
+      <c r="AS22" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A23" s="40">
         <v>22</v>
       </c>
@@ -4824,26 +4900,29 @@
       <c r="AL23" s="46">
         <v>1167.79</v>
       </c>
-      <c r="AM23" s="45">
+      <c r="AM23" s="27">
+        <v>0.78700000000000003</v>
+      </c>
+      <c r="AN23" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN23" s="50">
+      <c r="AO23" s="50">
         <v>3.7</v>
       </c>
-      <c r="AO23" s="45">
+      <c r="AP23" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP23" s="50">
+      <c r="AQ23" s="50">
         <v>3.742</v>
       </c>
-      <c r="AQ23" t="s">
+      <c r="AR23" t="s">
         <v>263</v>
       </c>
-      <c r="AR23" s="46">
+      <c r="AS23" s="46">
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A24" s="40">
         <v>23</v>
       </c>
@@ -4958,26 +5037,29 @@
       <c r="AL24" s="46">
         <v>727.90300000000002</v>
       </c>
-      <c r="AM24" s="45">
+      <c r="AM24" s="27">
+        <v>0.33200000000000002</v>
+      </c>
+      <c r="AN24" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN24" s="50">
+      <c r="AO24" s="50">
         <v>3.4860000000000002</v>
       </c>
-      <c r="AO24" s="45">
+      <c r="AP24" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP24" s="50">
+      <c r="AQ24" s="50">
         <v>3.6459999999999999</v>
       </c>
-      <c r="AQ24" s="42" t="s">
+      <c r="AR24" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="AR24" s="46">
+      <c r="AS24" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A25" s="40">
         <v>24</v>
       </c>
@@ -5092,26 +5174,29 @@
       <c r="AL25" s="46">
         <v>795.66200000000003</v>
       </c>
-      <c r="AM25" s="45">
+      <c r="AM25" s="27">
+        <v>0.34899999999999998</v>
+      </c>
+      <c r="AN25" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN25" s="50">
+      <c r="AO25" s="50">
         <v>3.51</v>
       </c>
-      <c r="AO25" s="45">
+      <c r="AP25" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP25" s="50">
+      <c r="AQ25" s="50">
         <v>3.6749999999999998</v>
       </c>
-      <c r="AQ25" t="s">
+      <c r="AR25" t="s">
         <v>259</v>
       </c>
-      <c r="AR25" s="46">
+      <c r="AS25" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A26" s="40">
         <v>25</v>
       </c>
@@ -5226,26 +5311,29 @@
       <c r="AL26" s="46" t="s">
         <v>259</v>
       </c>
-      <c r="AM26" s="45" t="s">
+      <c r="AM26" s="27" t="s">
         <v>259</v>
       </c>
-      <c r="AN26" s="50" t="s">
+      <c r="AN26" s="45" t="s">
         <v>259</v>
       </c>
-      <c r="AO26" s="45" t="s">
+      <c r="AO26" s="50" t="s">
         <v>259</v>
       </c>
-      <c r="AP26" s="50" t="s">
+      <c r="AP26" s="45" t="s">
         <v>259</v>
       </c>
-      <c r="AQ26" t="s">
+      <c r="AQ26" s="50" t="s">
         <v>259</v>
       </c>
-      <c r="AR26" s="46" t="s">
+      <c r="AR26" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="27" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AS26" s="46" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="27" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A27" s="40">
         <v>26</v>
       </c>
@@ -5360,26 +5448,29 @@
       <c r="AL27" s="46">
         <v>1745.1559999999999</v>
       </c>
-      <c r="AM27" s="45">
+      <c r="AM27" s="27">
+        <v>1.0669999999999999</v>
+      </c>
+      <c r="AN27" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN27" s="50">
+      <c r="AO27" s="50">
         <v>3.8010000000000002</v>
       </c>
-      <c r="AO27" s="45">
+      <c r="AP27" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP27" s="50">
+      <c r="AQ27" s="50">
         <v>3.694</v>
       </c>
-      <c r="AQ27" t="s">
+      <c r="AR27" t="s">
         <v>264</v>
       </c>
-      <c r="AR27" s="46">
+      <c r="AS27" s="46">
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A28" s="40">
         <v>27</v>
       </c>
@@ -5494,26 +5585,29 @@
       <c r="AL28" s="46">
         <v>1169.3810000000001</v>
       </c>
-      <c r="AM28" s="45">
+      <c r="AM28" s="27">
+        <v>0.54400000000000004</v>
+      </c>
+      <c r="AN28" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN28" s="50">
+      <c r="AO28" s="50">
         <v>3.629</v>
       </c>
-      <c r="AO28" s="45">
+      <c r="AP28" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP28" s="50">
+      <c r="AQ28" s="50">
         <v>3.7890000000000001</v>
       </c>
-      <c r="AQ28" t="s">
+      <c r="AR28" t="s">
         <v>259</v>
       </c>
-      <c r="AR28" s="46">
+      <c r="AS28" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A29" s="40">
         <v>28</v>
       </c>
@@ -5628,26 +5722,29 @@
       <c r="AL29" s="46">
         <v>1885.7059999999999</v>
       </c>
-      <c r="AM29" s="45">
+      <c r="AM29" s="27">
+        <v>1.397</v>
+      </c>
+      <c r="AN29" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN29" s="50">
+      <c r="AO29" s="50">
         <v>3.8719999999999999</v>
       </c>
-      <c r="AO29" s="45">
+      <c r="AP29" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP29" s="50">
+      <c r="AQ29" s="50">
         <v>3.9049999999999998</v>
       </c>
-      <c r="AQ29" t="s">
+      <c r="AR29" t="s">
         <v>264</v>
       </c>
-      <c r="AR29" s="46">
+      <c r="AS29" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A30" s="40">
         <v>29</v>
       </c>
@@ -5762,26 +5859,29 @@
       <c r="AL30" s="46">
         <v>1902</v>
       </c>
-      <c r="AM30" s="45">
+      <c r="AM30" s="27">
+        <v>2.7229999999999999</v>
+      </c>
+      <c r="AN30" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN30" s="50">
+      <c r="AO30" s="50">
         <v>4.1470000000000002</v>
       </c>
-      <c r="AO30" s="45">
+      <c r="AP30" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP30" s="50">
+      <c r="AQ30" s="50">
         <v>4.1920000000000002</v>
       </c>
-      <c r="AQ30" t="s">
+      <c r="AR30" t="s">
         <v>265</v>
       </c>
-      <c r="AR30" s="46">
+      <c r="AS30" s="46">
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A31" s="40">
         <v>30</v>
       </c>
@@ -5896,26 +5996,29 @@
       <c r="AL31" s="46">
         <v>760.072</v>
       </c>
-      <c r="AM31" s="45">
+      <c r="AM31" s="27">
+        <v>0.58799999999999997</v>
+      </c>
+      <c r="AN31" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN31" s="50">
+      <c r="AO31" s="50">
         <v>3.62</v>
       </c>
-      <c r="AO31" s="45">
+      <c r="AP31" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP31" s="50">
+      <c r="AQ31" s="50">
         <v>3.8039999999999998</v>
       </c>
-      <c r="AQ31" s="42" t="s">
+      <c r="AR31" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="AR31" s="46">
+      <c r="AS31" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A32" s="40">
         <v>31</v>
       </c>
@@ -6030,26 +6133,29 @@
       <c r="AL32" s="46">
         <v>685.81899999999996</v>
       </c>
-      <c r="AM32" s="45">
+      <c r="AM32" s="27">
+        <v>0.371</v>
+      </c>
+      <c r="AN32" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN32" s="50">
+      <c r="AO32" s="50">
         <v>3.5379999999999998</v>
       </c>
-      <c r="AO32" s="45">
+      <c r="AP32" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP32" s="50">
+      <c r="AQ32" s="50">
         <v>3.5209999999999999</v>
       </c>
-      <c r="AQ32" t="s">
+      <c r="AR32" t="s">
         <v>259</v>
       </c>
-      <c r="AR32" s="46">
+      <c r="AS32" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="33" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A33" s="40">
         <v>32</v>
       </c>
@@ -6164,26 +6270,29 @@
       <c r="AL33" s="46">
         <v>1997.3</v>
       </c>
-      <c r="AM33" s="45">
+      <c r="AM33" s="50">
+        <v>1301</v>
+      </c>
+      <c r="AN33" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN33" s="50">
+      <c r="AO33" s="50">
         <v>3.7730000000000001</v>
       </c>
-      <c r="AO33" s="45">
+      <c r="AP33" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP33" s="50">
+      <c r="AQ33" s="50">
         <v>3.9329999999999998</v>
       </c>
-      <c r="AQ33" t="s">
+      <c r="AR33" t="s">
         <v>264</v>
       </c>
-      <c r="AR33" s="46">
+      <c r="AS33" s="46">
         <v>8060</v>
       </c>
     </row>
-    <row r="34" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A34" s="40">
         <v>33</v>
       </c>
@@ -6298,26 +6407,29 @@
       <c r="AL34" s="46">
         <v>1213.203</v>
       </c>
-      <c r="AM34" s="45">
+      <c r="AM34" s="27">
+        <v>1.421</v>
+      </c>
+      <c r="AN34" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN34" s="50">
+      <c r="AO34" s="50">
         <v>3.8029999999999999</v>
       </c>
-      <c r="AO34" s="45">
+      <c r="AP34" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP34" s="50">
+      <c r="AQ34" s="50">
         <v>3.8290000000000002</v>
       </c>
-      <c r="AQ34" s="42" t="s">
+      <c r="AR34" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="AR34" s="46">
+      <c r="AS34" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="35" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A35" s="40">
         <v>34</v>
       </c>
@@ -6432,26 +6544,29 @@
       <c r="AL35" s="46">
         <v>1492.2660000000001</v>
       </c>
-      <c r="AM35" s="45">
+      <c r="AM35" s="27">
+        <v>2.0630000000000002</v>
+      </c>
+      <c r="AN35" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN35" s="50">
+      <c r="AO35" s="50">
         <v>4.0410000000000004</v>
       </c>
-      <c r="AO35" s="45">
+      <c r="AP35" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP35" s="50">
+      <c r="AQ35" s="50">
         <v>3.524</v>
       </c>
-      <c r="AQ35" s="42" t="s">
+      <c r="AR35" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="AR35" s="46">
+      <c r="AS35" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="36" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A36" s="40">
         <v>35</v>
       </c>
@@ -6566,26 +6681,29 @@
       <c r="AL36" s="46">
         <v>489.91899999999998</v>
       </c>
-      <c r="AM36" s="45">
+      <c r="AM36" s="27">
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="AN36" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN36" s="50">
+      <c r="AO36" s="50">
         <v>3.5430000000000001</v>
       </c>
-      <c r="AO36" s="45">
+      <c r="AP36" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP36" s="50">
+      <c r="AQ36" s="50">
         <v>3.7440000000000002</v>
       </c>
-      <c r="AQ36" s="42" t="s">
+      <c r="AR36" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="AR36" s="46">
+      <c r="AS36" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A37" s="40">
         <v>36</v>
       </c>
@@ -6700,26 +6818,29 @@
       <c r="AL37" s="46">
         <v>505.92200000000003</v>
       </c>
-      <c r="AM37" s="45">
+      <c r="AM37" s="27">
+        <v>0.26900000000000002</v>
+      </c>
+      <c r="AN37" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN37" s="50">
+      <c r="AO37" s="50">
         <v>3.4569999999999999</v>
       </c>
-      <c r="AO37" s="45">
+      <c r="AP37" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP37" s="50">
+      <c r="AQ37" s="50">
         <v>3.621</v>
       </c>
-      <c r="AQ37" s="42" t="s">
+      <c r="AR37" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="AR37" s="46">
+      <c r="AS37" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A38" s="40">
         <v>37</v>
       </c>
@@ -6834,26 +6955,29 @@
       <c r="AL38" s="46">
         <v>1560.482</v>
       </c>
-      <c r="AM38" s="45">
+      <c r="AM38" s="27">
+        <v>1.1359999999999999</v>
+      </c>
+      <c r="AN38" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN38" s="50">
+      <c r="AO38" s="50">
         <v>3.8410000000000002</v>
       </c>
-      <c r="AO38" s="45">
+      <c r="AP38" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP38" s="50">
+      <c r="AQ38" s="50">
         <v>3.8929999999999998</v>
       </c>
-      <c r="AQ38" s="42" t="s">
+      <c r="AR38" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="AR38" s="46">
+      <c r="AS38" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="39" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A39" s="40">
         <v>38</v>
       </c>
@@ -6968,26 +7092,29 @@
       <c r="AL39" s="46">
         <v>672.26199999999994</v>
       </c>
-      <c r="AM39" s="45">
+      <c r="AM39" s="27">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="AN39" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN39" s="50">
+      <c r="AO39" s="50">
         <v>3.556</v>
       </c>
-      <c r="AO39" s="45">
+      <c r="AP39" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP39" s="50">
+      <c r="AQ39" s="50">
         <v>3.544</v>
       </c>
-      <c r="AQ39" t="s">
+      <c r="AR39" t="s">
         <v>266</v>
       </c>
-      <c r="AR39" s="46">
+      <c r="AS39" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="40" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A40" s="40">
         <v>39</v>
       </c>
@@ -7102,26 +7229,29 @@
       <c r="AL40" s="46">
         <v>385.101</v>
       </c>
-      <c r="AM40" s="45">
+      <c r="AM40" s="27">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="AN40" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN40" s="49">
+      <c r="AO40" s="49">
         <v>3.5110000000000001</v>
       </c>
-      <c r="AO40" s="45">
+      <c r="AP40" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP40" s="49">
+      <c r="AQ40" s="49">
         <v>3.8929999999999998</v>
       </c>
-      <c r="AQ40" s="42" t="s">
+      <c r="AR40" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="AR40" s="46">
+      <c r="AS40" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="41" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A41" s="40">
         <v>40</v>
       </c>
@@ -7236,26 +7366,29 @@
       <c r="AL41" s="48">
         <v>1375.145</v>
       </c>
-      <c r="AM41" s="45">
+      <c r="AM41" s="27">
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="AN41" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN41" s="49">
+      <c r="AO41" s="49">
         <v>3.6269999999999998</v>
       </c>
-      <c r="AO41" s="45">
+      <c r="AP41" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP41" s="49">
+      <c r="AQ41" s="49">
         <v>3.774</v>
       </c>
-      <c r="AQ41" s="42" t="s">
+      <c r="AR41" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="AR41" s="46">
+      <c r="AS41" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="42" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A42" s="40">
         <v>41</v>
       </c>
@@ -7370,27 +7503,30 @@
       <c r="AL42" s="46">
         <v>919.31</v>
       </c>
-      <c r="AM42" s="45">
+      <c r="AM42" s="27">
+        <v>0.92600000000000005</v>
+      </c>
+      <c r="AN42" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN42" s="49">
+      <c r="AO42" s="49">
         <v>3.681</v>
       </c>
-      <c r="AO42" s="45">
+      <c r="AP42" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP42" s="49">
+      <c r="AQ42" s="49">
         <v>3.7949999999999999</v>
       </c>
-      <c r="AQ42" s="42" t="s">
+      <c r="AR42" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="AR42" s="46">
+      <c r="AS42" s="46">
         <v>80</v>
       </c>
-      <c r="AW42" s="11"/>
-    </row>
-    <row r="43" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AX42" s="11"/>
+    </row>
+    <row r="43" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A43" s="40">
         <v>42</v>
       </c>
@@ -7505,27 +7641,30 @@
       <c r="AL43" s="46">
         <v>1030.7909999999999</v>
       </c>
-      <c r="AM43" s="45">
+      <c r="AM43" s="27">
+        <v>1.222</v>
+      </c>
+      <c r="AN43" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN43" s="49">
+      <c r="AO43" s="49">
         <v>3.7919999999999998</v>
       </c>
-      <c r="AO43" s="45">
+      <c r="AP43" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP43" s="49">
+      <c r="AQ43" s="49">
         <v>4.4669999999999996</v>
       </c>
-      <c r="AQ43" s="42" t="s">
+      <c r="AR43" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="AR43" s="46">
+      <c r="AS43" s="46">
         <v>80</v>
       </c>
-      <c r="AW43" s="11"/>
-    </row>
-    <row r="44" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AX43" s="11"/>
+    </row>
+    <row r="44" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A44" s="40">
         <v>43</v>
       </c>
@@ -7640,27 +7779,30 @@
       <c r="AL44" s="46">
         <v>306.67899999999997</v>
       </c>
-      <c r="AM44" s="45">
+      <c r="AM44" s="27">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="AN44" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN44" s="49">
+      <c r="AO44" s="49">
         <v>3.456</v>
       </c>
-      <c r="AO44" s="45">
+      <c r="AP44" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP44" s="49">
+      <c r="AQ44" s="49">
         <v>3.5630000000000002</v>
       </c>
-      <c r="AQ44" s="42" t="s">
+      <c r="AR44" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="AR44" s="46">
+      <c r="AS44" s="46">
         <v>80</v>
       </c>
-      <c r="AW44" s="11"/>
-    </row>
-    <row r="45" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AX44" s="11"/>
+    </row>
+    <row r="45" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A45" s="40">
         <v>44</v>
       </c>
@@ -7775,27 +7917,30 @@
       <c r="AL45" s="46">
         <v>785.101</v>
       </c>
-      <c r="AM45" s="45">
+      <c r="AM45" s="27">
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="AN45" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN45" s="49">
+      <c r="AO45" s="49">
         <v>3.5350000000000001</v>
       </c>
-      <c r="AO45" s="45">
+      <c r="AP45" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP45" s="49">
+      <c r="AQ45" s="49">
         <v>3.5249999999999999</v>
       </c>
-      <c r="AQ45" s="42" t="s">
+      <c r="AR45" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="AR45" s="46">
+      <c r="AS45" s="46">
         <v>80</v>
       </c>
-      <c r="AW45" s="11"/>
-    </row>
-    <row r="46" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AX45" s="11"/>
+    </row>
+    <row r="46" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A46" s="40">
         <v>45</v>
       </c>
@@ -7910,26 +8055,29 @@
       <c r="AL46" s="46">
         <v>607.05399999999997</v>
       </c>
-      <c r="AM46" s="45">
+      <c r="AM46" s="27">
+        <v>0.54100000000000004</v>
+      </c>
+      <c r="AN46" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN46" s="49">
+      <c r="AO46" s="49">
         <v>3.585</v>
       </c>
-      <c r="AO46" s="45">
+      <c r="AP46" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP46" s="49">
+      <c r="AQ46" s="49">
         <v>3.516</v>
       </c>
-      <c r="AQ46" s="42" t="s">
+      <c r="AR46" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="AR46" s="46">
+      <c r="AS46" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="47" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A47" s="40">
         <v>46</v>
       </c>
@@ -8044,26 +8192,29 @@
       <c r="AL47" s="46">
         <v>397.02800000000002</v>
       </c>
-      <c r="AM47" s="45">
+      <c r="AM47" s="27">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="AN47" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN47" s="49">
+      <c r="AO47" s="49">
         <v>3.5720000000000001</v>
       </c>
-      <c r="AO47" s="45">
+      <c r="AP47" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP47" s="49">
+      <c r="AQ47" s="49">
         <v>3.51</v>
       </c>
-      <c r="AQ47" s="42" t="s">
+      <c r="AR47" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="AR47" s="46">
+      <c r="AS47" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="48" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A48" s="40">
         <v>47</v>
       </c>
@@ -8178,26 +8329,29 @@
       <c r="AL48" s="46">
         <v>1026.5519999999999</v>
       </c>
-      <c r="AM48" s="45">
+      <c r="AM48" s="27">
+        <v>0.47899999999999998</v>
+      </c>
+      <c r="AN48" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN48" s="49">
+      <c r="AO48" s="49">
         <v>3.6869999999999998</v>
       </c>
-      <c r="AO48" s="45">
+      <c r="AP48" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP48" s="49">
+      <c r="AQ48" s="49">
         <v>3.7850000000000001</v>
       </c>
-      <c r="AQ48" s="42" t="s">
+      <c r="AR48" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="AR48" s="46">
+      <c r="AS48" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="49" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A49" s="40">
         <v>48</v>
       </c>
@@ -8312,26 +8466,29 @@
       <c r="AL49" s="46">
         <v>488.82600000000002</v>
       </c>
-      <c r="AM49" s="45">
+      <c r="AM49" s="27">
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="AN49" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN49" s="49">
+      <c r="AO49" s="49">
         <v>3.5249999999999999</v>
       </c>
-      <c r="AO49" s="45">
+      <c r="AP49" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP49" s="49">
+      <c r="AQ49" s="49">
         <v>3.504</v>
       </c>
-      <c r="AQ49" s="42" t="s">
+      <c r="AR49" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="AR49" s="46">
+      <c r="AS49" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="50" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A50" s="40">
         <v>49</v>
       </c>
@@ -8446,26 +8603,29 @@
       <c r="AL50" s="46">
         <v>1290.2819999999999</v>
       </c>
-      <c r="AM50" s="45">
+      <c r="AM50" s="27">
+        <v>1.159</v>
+      </c>
+      <c r="AN50" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN50" s="50">
+      <c r="AO50" s="50">
         <v>3.7269999999999999</v>
       </c>
-      <c r="AO50" s="45">
+      <c r="AP50" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP50" s="50">
+      <c r="AQ50" s="50">
         <v>3.681</v>
       </c>
-      <c r="AQ50" t="s">
+      <c r="AR50" t="s">
         <v>262</v>
       </c>
-      <c r="AR50" s="46">
+      <c r="AS50" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="51" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A51" s="40">
         <v>50</v>
       </c>
@@ -8580,26 +8740,29 @@
       <c r="AL51" s="46">
         <v>614.70299999999997</v>
       </c>
-      <c r="AM51" s="45">
+      <c r="AM51" s="27">
+        <v>0.58699999999999997</v>
+      </c>
+      <c r="AN51" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN51" s="49">
+      <c r="AO51" s="49">
         <v>3.5409999999999999</v>
       </c>
-      <c r="AO51" s="45">
+      <c r="AP51" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP51" s="49">
+      <c r="AQ51" s="49">
         <v>3.5870000000000002</v>
       </c>
-      <c r="AQ51" s="42" t="s">
+      <c r="AR51" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="AR51" s="46">
+      <c r="AS51" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="52" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A52" s="40">
         <v>51</v>
       </c>
@@ -8714,26 +8877,29 @@
       <c r="AL52" s="46">
         <v>362.14</v>
       </c>
-      <c r="AM52" s="45">
+      <c r="AM52" s="27">
+        <v>0.31</v>
+      </c>
+      <c r="AN52" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN52" s="49">
+      <c r="AO52" s="49">
         <v>3.5030000000000001</v>
       </c>
-      <c r="AO52" s="45">
+      <c r="AP52" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP52" s="49">
+      <c r="AQ52" s="49">
         <v>3.621</v>
       </c>
-      <c r="AQ52" s="42" t="s">
+      <c r="AR52" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="AR52" s="46">
+      <c r="AS52" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="53" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A53" s="40">
         <v>52</v>
       </c>
@@ -8848,26 +9014,29 @@
       <c r="AL53" s="46">
         <v>942.29499999999996</v>
       </c>
-      <c r="AM53" s="45">
+      <c r="AM53" s="27">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="AN53" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN53" s="49">
+      <c r="AO53" s="49">
         <v>3.6339999999999999</v>
       </c>
-      <c r="AO53" s="45">
+      <c r="AP53" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP53" s="49">
+      <c r="AQ53" s="49">
         <v>3.637</v>
       </c>
-      <c r="AQ53" s="42" t="s">
+      <c r="AR53" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="AR53" s="46">
+      <c r="AS53" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="54" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A54" s="40">
         <v>53</v>
       </c>
@@ -8982,26 +9151,29 @@
       <c r="AL54" s="46">
         <v>703.31100000000004</v>
       </c>
-      <c r="AM54" s="45">
+      <c r="AM54" s="27">
+        <v>0.47899999999999998</v>
+      </c>
+      <c r="AN54" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN54" s="49">
+      <c r="AO54" s="49">
         <v>3.5680000000000001</v>
       </c>
-      <c r="AO54" s="45">
+      <c r="AP54" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP54" s="49">
+      <c r="AQ54" s="49">
         <v>3.5630000000000002</v>
       </c>
-      <c r="AQ54" s="42" t="s">
+      <c r="AR54" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="AR54" s="46">
+      <c r="AS54" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="55" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A55" s="40">
         <v>54</v>
       </c>
@@ -9116,26 +9288,29 @@
       <c r="AL55" s="46">
         <v>1101.4670000000001</v>
       </c>
-      <c r="AM55" s="45">
+      <c r="AM55" s="27">
+        <v>1.1739999999999999</v>
+      </c>
+      <c r="AN55" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN55" s="49">
+      <c r="AO55" s="49">
         <v>3.742</v>
       </c>
-      <c r="AO55" s="45">
+      <c r="AP55" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP55" s="49">
+      <c r="AQ55" s="49">
         <v>3.9249999999999998</v>
       </c>
-      <c r="AQ55" s="42" t="s">
+      <c r="AR55" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="AR55" s="46">
+      <c r="AS55" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="56" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A56" s="40">
         <v>55</v>
       </c>
@@ -9250,26 +9425,29 @@
       <c r="AL56" s="46">
         <v>796.21900000000005</v>
       </c>
-      <c r="AM56" s="45">
+      <c r="AM56" s="27">
+        <v>0.38800000000000001</v>
+      </c>
+      <c r="AN56" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN56" s="49">
+      <c r="AO56" s="49">
         <v>3.51</v>
       </c>
-      <c r="AO56" s="45">
+      <c r="AP56" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP56" s="49">
+      <c r="AQ56" s="49">
         <v>3.6749999999999998</v>
       </c>
-      <c r="AQ56" s="42" t="s">
+      <c r="AR56" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="AR56" s="46">
+      <c r="AS56" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="57" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A57" s="40">
         <v>56</v>
       </c>
@@ -9384,26 +9562,29 @@
       <c r="AL57" s="46">
         <v>1404.249</v>
       </c>
-      <c r="AM57" s="45">
+      <c r="AM57" s="27">
+        <v>0.88900000000000001</v>
+      </c>
+      <c r="AN57" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN57" s="49">
+      <c r="AO57" s="49">
         <v>3.6389999999999998</v>
       </c>
-      <c r="AO57" s="45">
+      <c r="AP57" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP57" s="49">
+      <c r="AQ57" s="49">
         <v>3.9039999999999999</v>
       </c>
-      <c r="AQ57" t="s">
+      <c r="AR57" t="s">
         <v>262</v>
       </c>
-      <c r="AR57" s="46">
+      <c r="AS57" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="58" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A58" s="40">
         <v>57</v>
       </c>
@@ -9518,26 +9699,29 @@
       <c r="AL58" s="46">
         <v>890.17700000000002</v>
       </c>
-      <c r="AM58" s="45">
+      <c r="AM58" s="27">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="AN58" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN58" s="49">
+      <c r="AO58" s="49">
         <v>3.665</v>
       </c>
-      <c r="AO58" s="45">
+      <c r="AP58" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP58" s="49">
+      <c r="AQ58" s="49">
         <v>3.613</v>
       </c>
-      <c r="AQ58" t="s">
+      <c r="AR58" t="s">
         <v>263</v>
       </c>
-      <c r="AR58" s="46">
+      <c r="AS58" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="59" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A59" s="40">
         <v>58</v>
       </c>
@@ -9652,26 +9836,29 @@
       <c r="AL59" s="46">
         <v>1589.546</v>
       </c>
-      <c r="AM59" s="45">
+      <c r="AM59" s="27">
+        <v>1.298</v>
+      </c>
+      <c r="AN59" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN59" s="49">
+      <c r="AO59" s="49">
         <v>3.8010000000000002</v>
       </c>
-      <c r="AO59" s="45">
+      <c r="AP59" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP59" s="49">
+      <c r="AQ59" s="49">
         <v>3.8490000000000002</v>
       </c>
-      <c r="AQ59" s="42" t="s">
+      <c r="AR59" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="AR59" s="46">
+      <c r="AS59" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="60" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A60" s="40">
         <v>59</v>
       </c>
@@ -9786,26 +9973,29 @@
       <c r="AL60" s="46">
         <v>448.74099999999999</v>
       </c>
-      <c r="AM60" s="45">
+      <c r="AM60" s="27">
+        <v>0.23300000000000001</v>
+      </c>
+      <c r="AN60" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN60" s="49">
+      <c r="AO60" s="49">
         <v>3.4849999999999999</v>
       </c>
-      <c r="AO60" s="45">
+      <c r="AP60" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP60" s="49">
+      <c r="AQ60" s="49">
         <v>3.8730000000000002</v>
       </c>
-      <c r="AQ60" s="42" t="s">
+      <c r="AR60" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="AR60" s="46">
+      <c r="AS60" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="61" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A61" s="40">
         <v>60</v>
       </c>
@@ -9920,26 +10110,29 @@
       <c r="AL61" s="46">
         <v>1668.8420000000001</v>
       </c>
-      <c r="AM61" s="45">
+      <c r="AM61" s="27">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="AN61" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN61" s="49">
+      <c r="AO61" s="49">
         <v>3.673</v>
       </c>
-      <c r="AO61" s="45">
+      <c r="AP61" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP61" s="49">
+      <c r="AQ61" s="49">
         <v>3.976</v>
       </c>
-      <c r="AQ61" t="s">
+      <c r="AR61" t="s">
         <v>264</v>
       </c>
-      <c r="AR61" s="46">
+      <c r="AS61" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="62" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A62" s="40">
         <v>61</v>
       </c>
@@ -10054,26 +10247,29 @@
       <c r="AL62" s="46">
         <v>918.48199999999997</v>
       </c>
-      <c r="AM62" s="45">
+      <c r="AM62" s="27">
+        <v>0.64800000000000002</v>
+      </c>
+      <c r="AN62" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN62" s="49">
+      <c r="AO62" s="49">
         <v>3.5579999999999998</v>
       </c>
-      <c r="AO62" s="45">
+      <c r="AP62" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP62" s="49">
+      <c r="AQ62" s="49">
         <v>3.5459999999999998</v>
       </c>
-      <c r="AQ62" t="s">
+      <c r="AR62" t="s">
         <v>259</v>
       </c>
-      <c r="AR62" s="46">
+      <c r="AS62" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="63" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A63" s="40">
         <v>62</v>
       </c>
@@ -10188,26 +10384,29 @@
       <c r="AL63" s="46">
         <v>1202.396</v>
       </c>
-      <c r="AM63" s="45">
+      <c r="AM63" s="27">
+        <v>0.72199999999999998</v>
+      </c>
+      <c r="AN63" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN63" s="49">
+      <c r="AO63" s="49">
         <v>3.746</v>
       </c>
-      <c r="AO63" s="45">
+      <c r="AP63" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP63" s="49">
+      <c r="AQ63" s="49">
         <v>3.7709999999999999</v>
       </c>
-      <c r="AQ63" t="s">
+      <c r="AR63" t="s">
         <v>262</v>
       </c>
-      <c r="AR63" s="46">
+      <c r="AS63" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="64" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A64" s="40">
         <v>63</v>
       </c>
@@ -10322,26 +10521,29 @@
       <c r="AL64" s="46">
         <v>1212.846</v>
       </c>
-      <c r="AM64" s="45">
+      <c r="AM64" s="27">
+        <v>0.97299999999999998</v>
+      </c>
+      <c r="AN64" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN64" s="49">
+      <c r="AO64" s="49">
         <v>3.7519999999999998</v>
       </c>
-      <c r="AO64" s="45">
+      <c r="AP64" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP64" s="49">
+      <c r="AQ64" s="49">
         <v>4.18</v>
       </c>
-      <c r="AQ64" t="s">
+      <c r="AR64" t="s">
         <v>267</v>
       </c>
-      <c r="AR64" s="46">
+      <c r="AS64" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="65" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A65" s="40">
         <v>64</v>
       </c>
@@ -10456,26 +10658,29 @@
       <c r="AL65" s="46">
         <v>917.59299999999996</v>
       </c>
-      <c r="AM65" s="45">
+      <c r="AM65" s="27">
+        <v>0.43</v>
+      </c>
+      <c r="AN65" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN65" s="49">
+      <c r="AO65" s="49">
         <v>3.573</v>
       </c>
-      <c r="AO65" s="45">
+      <c r="AP65" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP65" s="49">
+      <c r="AQ65" s="49">
         <v>3.6150000000000002</v>
       </c>
-      <c r="AQ65" t="s">
+      <c r="AR65" t="s">
         <v>259</v>
       </c>
-      <c r="AR65" s="46">
+      <c r="AS65" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="66" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A66" s="40">
         <v>65</v>
       </c>
@@ -10590,26 +10795,29 @@
       <c r="AL66" s="46">
         <v>1081.271</v>
       </c>
-      <c r="AM66" s="45">
+      <c r="AM66" s="27">
+        <v>0.91300000000000003</v>
+      </c>
+      <c r="AN66" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN66" s="49">
+      <c r="AO66" s="49">
         <v>3.7519999999999998</v>
       </c>
-      <c r="AO66" s="45">
+      <c r="AP66" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP66" s="49">
+      <c r="AQ66" s="49">
         <v>3.5819999999999999</v>
       </c>
-      <c r="AQ66" t="s">
+      <c r="AR66" t="s">
         <v>259</v>
       </c>
-      <c r="AR66" s="46">
+      <c r="AS66" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="67" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A67" s="40">
         <v>66</v>
       </c>
@@ -10724,26 +10932,29 @@
       <c r="AL67" s="46">
         <v>790.43</v>
       </c>
-      <c r="AM67" s="45">
+      <c r="AM67" s="27">
+        <v>0.74299999999999999</v>
+      </c>
+      <c r="AN67" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN67" s="49">
+      <c r="AO67" s="49">
         <v>3.722</v>
       </c>
-      <c r="AO67" s="45">
+      <c r="AP67" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP67" s="49">
+      <c r="AQ67" s="49">
         <v>3.621</v>
       </c>
-      <c r="AQ67" t="s">
+      <c r="AR67" t="s">
         <v>259</v>
       </c>
-      <c r="AR67" s="46">
+      <c r="AS67" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="68" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A68" s="40">
         <v>67</v>
       </c>
@@ -10858,26 +11069,29 @@
       <c r="AL68" s="46">
         <v>626.20000000000005</v>
       </c>
-      <c r="AM68" s="45">
+      <c r="AM68" s="27">
+        <v>0.249</v>
+      </c>
+      <c r="AN68" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN68" s="49">
+      <c r="AO68" s="49">
         <v>3.51</v>
       </c>
-      <c r="AO68" s="45">
+      <c r="AP68" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP68" s="49">
+      <c r="AQ68" s="49">
         <v>3.7130000000000001</v>
       </c>
-      <c r="AQ68" t="s">
+      <c r="AR68" t="s">
         <v>259</v>
       </c>
-      <c r="AR68" s="46">
+      <c r="AS68" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="69" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A69" s="40">
         <v>68</v>
       </c>
@@ -10992,26 +11206,29 @@
       <c r="AL69" s="46">
         <v>1691</v>
       </c>
-      <c r="AM69" s="45">
+      <c r="AM69" s="27">
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="AN69" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN69" s="49">
+      <c r="AO69" s="49">
         <v>3.7530000000000001</v>
       </c>
-      <c r="AO69" s="45">
+      <c r="AP69" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP69" s="49">
+      <c r="AQ69" s="49">
         <v>3.613</v>
       </c>
-      <c r="AQ69" t="s">
+      <c r="AR69" t="s">
         <v>259</v>
       </c>
-      <c r="AR69" s="46">
+      <c r="AS69" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="70" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A70" s="40">
         <v>69</v>
       </c>
@@ -11126,26 +11343,29 @@
       <c r="AL70" s="46">
         <v>569</v>
       </c>
-      <c r="AM70" s="45">
+      <c r="AM70" s="27">
+        <v>0.307</v>
+      </c>
+      <c r="AN70" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN70" s="49">
+      <c r="AO70" s="49">
         <v>3.55</v>
       </c>
-      <c r="AO70" s="45">
+      <c r="AP70" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP70" s="49">
+      <c r="AQ70" s="49">
         <v>3.7360000000000002</v>
       </c>
-      <c r="AQ70" t="s">
+      <c r="AR70" t="s">
         <v>259</v>
       </c>
-      <c r="AR70" s="46">
+      <c r="AS70" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="71" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A71" s="40">
         <v>70</v>
       </c>
@@ -11260,26 +11480,29 @@
       <c r="AL71" s="46">
         <v>972</v>
       </c>
-      <c r="AM71" s="45">
+      <c r="AM71" s="27">
+        <v>1.248</v>
+      </c>
+      <c r="AN71" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN71" s="49">
+      <c r="AO71" s="49">
         <v>3.702</v>
       </c>
-      <c r="AO71" s="45">
+      <c r="AP71" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP71" s="49">
+      <c r="AQ71" s="49">
         <v>3.823</v>
       </c>
-      <c r="AQ71" t="s">
+      <c r="AR71" t="s">
         <v>264</v>
       </c>
-      <c r="AR71" s="46">
+      <c r="AS71" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="72" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A72" s="40">
         <v>71</v>
       </c>
@@ -11394,26 +11617,29 @@
       <c r="AL72" s="46">
         <v>1581</v>
       </c>
-      <c r="AM72" s="45">
+      <c r="AM72" s="27">
+        <v>1.111</v>
+      </c>
+      <c r="AN72" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN72" s="49">
+      <c r="AO72" s="49">
         <v>3.706</v>
       </c>
-      <c r="AO72" s="45">
+      <c r="AP72" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP72" s="49">
+      <c r="AQ72" s="49">
         <v>3.8180000000000001</v>
       </c>
-      <c r="AQ72" t="s">
+      <c r="AR72" t="s">
         <v>259</v>
       </c>
-      <c r="AR72" s="46">
+      <c r="AS72" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="73" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A73" s="40">
         <v>72</v>
       </c>
@@ -11528,26 +11754,29 @@
       <c r="AL73" s="46">
         <v>830</v>
       </c>
-      <c r="AM73" s="45">
+      <c r="AM73" s="27">
+        <v>0.39700000000000002</v>
+      </c>
+      <c r="AN73" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN73" s="49">
+      <c r="AO73" s="49">
         <v>3.5840000000000001</v>
       </c>
-      <c r="AO73" s="45">
+      <c r="AP73" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP73" s="49">
+      <c r="AQ73" s="49">
         <v>3.8759999999999999</v>
       </c>
-      <c r="AQ73" t="s">
+      <c r="AR73" t="s">
         <v>259</v>
       </c>
-      <c r="AR73" s="46">
+      <c r="AS73" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="74" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A74" s="40">
         <v>73</v>
       </c>
@@ -11662,26 +11891,29 @@
       <c r="AL74" s="46">
         <v>981</v>
       </c>
-      <c r="AM74" s="45">
+      <c r="AM74" s="27">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="AN74" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN74" s="49">
+      <c r="AO74" s="49">
         <v>3.6269999999999998</v>
       </c>
-      <c r="AO74" s="45">
+      <c r="AP74" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP74" s="49">
+      <c r="AQ74" s="49">
         <v>3.7040000000000002</v>
       </c>
-      <c r="AQ74" t="s">
+      <c r="AR74" t="s">
         <v>259</v>
       </c>
-      <c r="AR74" s="46">
+      <c r="AS74" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="75" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A75" s="40">
         <v>74</v>
       </c>
@@ -11796,26 +12028,29 @@
       <c r="AL75" s="46">
         <v>813</v>
       </c>
-      <c r="AM75" s="45">
+      <c r="AM75" s="27">
+        <v>0.72099999999999997</v>
+      </c>
+      <c r="AN75" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN75" s="49">
+      <c r="AO75" s="49">
         <v>3.681</v>
       </c>
-      <c r="AO75" s="45">
+      <c r="AP75" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP75" s="49">
+      <c r="AQ75" s="49">
         <v>3.738</v>
       </c>
-      <c r="AQ75" t="s">
+      <c r="AR75" t="s">
         <v>259</v>
       </c>
-      <c r="AR75" s="46">
+      <c r="AS75" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="76" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A76" s="40">
         <v>75</v>
       </c>
@@ -11930,26 +12165,29 @@
       <c r="AL76" s="46">
         <v>2015</v>
       </c>
-      <c r="AM76" s="45">
+      <c r="AM76" s="27">
+        <v>0.755</v>
+      </c>
+      <c r="AN76" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN76" s="49">
+      <c r="AO76" s="49">
         <v>3.8359999999999999</v>
       </c>
-      <c r="AO76" s="45">
+      <c r="AP76" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP76" s="49">
+      <c r="AQ76" s="49">
         <v>4.1509999999999998</v>
       </c>
-      <c r="AQ76" t="s">
+      <c r="AR76" t="s">
         <v>259</v>
       </c>
-      <c r="AR76" s="46">
+      <c r="AS76" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="77" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A77" s="40">
         <v>76</v>
       </c>
@@ -12064,26 +12302,29 @@
       <c r="AL77" s="46">
         <v>897</v>
       </c>
-      <c r="AM77" s="45">
+      <c r="AM77" s="27">
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="AN77" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN77" s="49">
+      <c r="AO77" s="49">
         <v>3.57</v>
       </c>
-      <c r="AO77" s="45">
+      <c r="AP77" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP77" s="49">
+      <c r="AQ77" s="49">
         <v>3.7559999999999998</v>
       </c>
-      <c r="AQ77" t="s">
+      <c r="AR77" t="s">
         <v>264</v>
       </c>
-      <c r="AR77" s="46">
+      <c r="AS77" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="78" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A78" s="40">
         <v>77</v>
       </c>
@@ -12198,26 +12439,29 @@
       <c r="AL78" s="46">
         <v>1668</v>
       </c>
-      <c r="AM78" s="45">
+      <c r="AM78" s="27">
+        <v>0.70599999999999996</v>
+      </c>
+      <c r="AN78" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN78" s="49">
+      <c r="AO78" s="49">
         <v>3.7629999999999999</v>
       </c>
-      <c r="AO78" s="45">
+      <c r="AP78" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP78" s="49">
+      <c r="AQ78" s="49">
         <v>3.585</v>
       </c>
-      <c r="AQ78" t="s">
+      <c r="AR78" t="s">
         <v>262</v>
       </c>
-      <c r="AR78" s="46">
+      <c r="AS78" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="79" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A79" s="40">
         <v>78</v>
       </c>
@@ -12332,26 +12576,29 @@
       <c r="AL79" s="46">
         <v>1160</v>
       </c>
-      <c r="AM79" s="45">
+      <c r="AM79" s="27">
+        <v>1.929</v>
+      </c>
+      <c r="AN79" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN79" s="49">
+      <c r="AO79" s="49">
         <v>3.8959999999999999</v>
       </c>
-      <c r="AO79" s="45">
+      <c r="AP79" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP79" s="49">
+      <c r="AQ79" s="49">
         <v>3.7810000000000001</v>
       </c>
-      <c r="AQ79" t="s">
+      <c r="AR79" t="s">
         <v>264</v>
       </c>
-      <c r="AR79" s="46">
+      <c r="AS79" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="80" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A80" s="40">
         <v>79</v>
       </c>
@@ -12466,26 +12713,29 @@
       <c r="AL80" s="46">
         <v>858</v>
       </c>
-      <c r="AM80" s="45">
+      <c r="AM80" s="27">
+        <v>0.51800000000000002</v>
+      </c>
+      <c r="AN80" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN80" s="49">
+      <c r="AO80" s="49">
         <v>3.6139999999999999</v>
       </c>
-      <c r="AO80" s="45">
+      <c r="AP80" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP80" s="49">
+      <c r="AQ80" s="49">
         <v>3.9449999999999998</v>
       </c>
-      <c r="AQ80" t="s">
+      <c r="AR80" t="s">
         <v>259</v>
       </c>
-      <c r="AR80" s="46">
+      <c r="AS80" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="81" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A81" s="40">
         <v>80</v>
       </c>
@@ -12600,26 +12850,29 @@
       <c r="AL81" s="46">
         <v>2256</v>
       </c>
-      <c r="AM81" s="45">
+      <c r="AM81" s="27">
+        <v>1.028</v>
+      </c>
+      <c r="AN81" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN81" s="49">
+      <c r="AO81" s="49">
         <v>3.6859999999999999</v>
       </c>
-      <c r="AO81" s="45">
+      <c r="AP81" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP81" s="49">
+      <c r="AQ81" s="49">
         <v>3.9169999999999998</v>
       </c>
-      <c r="AQ81" t="s">
+      <c r="AR81" t="s">
         <v>259</v>
       </c>
-      <c r="AR81" s="46">
+      <c r="AS81" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A82" s="40">
         <v>81</v>
       </c>
@@ -12734,26 +12987,29 @@
       <c r="AL82" s="46">
         <v>911</v>
       </c>
-      <c r="AM82" s="45">
+      <c r="AM82" s="27">
+        <v>0.752</v>
+      </c>
+      <c r="AN82" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN82" s="49">
+      <c r="AO82" s="49">
         <v>3.5720000000000001</v>
       </c>
-      <c r="AO82" s="45">
+      <c r="AP82" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP82" s="49">
+      <c r="AQ82" s="49">
         <v>3.6869999999999998</v>
       </c>
-      <c r="AQ82" t="s">
+      <c r="AR82" t="s">
         <v>259</v>
       </c>
-      <c r="AR82" s="46">
+      <c r="AS82" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A83" s="40">
         <v>82</v>
       </c>
@@ -12868,26 +13124,29 @@
       <c r="AL83" s="46">
         <v>1132</v>
       </c>
-      <c r="AM83" s="45">
+      <c r="AM83" s="27">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="AN83" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN83" s="49">
+      <c r="AO83" s="49">
         <v>3.5760000000000001</v>
       </c>
-      <c r="AO83" s="45">
+      <c r="AP83" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP83" s="49">
+      <c r="AQ83" s="49">
         <v>4.0529999999999999</v>
       </c>
-      <c r="AQ83" t="s">
+      <c r="AR83" t="s">
         <v>259</v>
       </c>
-      <c r="AR83" s="46">
+      <c r="AS83" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="84" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A84" s="40">
         <v>83</v>
       </c>
@@ -13002,26 +13261,29 @@
       <c r="AL84" s="46">
         <v>1463</v>
       </c>
-      <c r="AM84" s="45">
+      <c r="AM84" s="27">
+        <v>0.94599999999999995</v>
+      </c>
+      <c r="AN84" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN84" s="49">
+      <c r="AO84" s="49">
         <v>3.746</v>
       </c>
-      <c r="AO84" s="45">
+      <c r="AP84" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP84" s="49">
+      <c r="AQ84" s="49">
         <v>3.6240000000000001</v>
       </c>
-      <c r="AQ84" t="s">
+      <c r="AR84" t="s">
         <v>259</v>
       </c>
-      <c r="AR84" s="46">
+      <c r="AS84" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="85" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A85" s="40">
         <v>84</v>
       </c>
@@ -13136,26 +13398,29 @@
       <c r="AL85" s="46">
         <v>712</v>
       </c>
-      <c r="AM85" s="45">
+      <c r="AM85" s="27">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="AN85" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN85" s="49">
+      <c r="AO85" s="49">
         <v>3.5</v>
       </c>
-      <c r="AO85" s="45">
+      <c r="AP85" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP85" s="49">
+      <c r="AQ85" s="49">
         <v>3.8610000000000002</v>
       </c>
-      <c r="AQ85" t="s">
+      <c r="AR85" t="s">
         <v>259</v>
       </c>
-      <c r="AR85" s="46">
+      <c r="AS85" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="86" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A86" s="40">
         <v>85</v>
       </c>
@@ -13270,26 +13535,29 @@
       <c r="AL86" s="46">
         <v>719</v>
       </c>
-      <c r="AM86" s="45">
+      <c r="AM86" s="27">
+        <v>0.71899999999999997</v>
+      </c>
+      <c r="AN86" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN86" s="49">
+      <c r="AO86" s="49">
         <v>3.665</v>
       </c>
-      <c r="AO86" s="45">
+      <c r="AP86" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP86" s="49">
+      <c r="AQ86" s="49">
         <v>3.5779999999999998</v>
       </c>
-      <c r="AQ86" t="s">
+      <c r="AR86" t="s">
         <v>259</v>
       </c>
-      <c r="AR86" s="46">
+      <c r="AS86" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="87" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A87" s="40">
         <v>86</v>
       </c>
@@ -13404,26 +13672,29 @@
       <c r="AL87" s="46">
         <v>1731</v>
       </c>
-      <c r="AM87" s="45">
+      <c r="AM87" s="27">
+        <v>0.6</v>
+      </c>
+      <c r="AN87" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN87" s="49">
+      <c r="AO87" s="49">
         <v>3.645</v>
       </c>
-      <c r="AO87" s="45">
+      <c r="AP87" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP87" s="49">
+      <c r="AQ87" s="49">
         <v>3.58</v>
       </c>
-      <c r="AQ87" t="s">
+      <c r="AR87" t="s">
         <v>259</v>
       </c>
-      <c r="AR87" s="46">
+      <c r="AS87" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="88" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A88" s="40">
         <v>87</v>
       </c>
@@ -13538,26 +13809,29 @@
       <c r="AL88" s="46">
         <v>508</v>
       </c>
-      <c r="AM88" s="45">
+      <c r="AM88" s="27">
+        <v>0.40200000000000002</v>
+      </c>
+      <c r="AN88" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN88" s="49">
+      <c r="AO88" s="49">
         <v>3.5529999999999999</v>
       </c>
-      <c r="AO88" s="45">
+      <c r="AP88" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP88" s="49">
+      <c r="AQ88" s="49">
         <v>3.5139999999999998</v>
       </c>
-      <c r="AQ88" t="s">
+      <c r="AR88" t="s">
         <v>259</v>
       </c>
-      <c r="AR88" s="46">
+      <c r="AS88" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="89" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A89" s="40">
         <v>88</v>
       </c>
@@ -13672,26 +13946,29 @@
       <c r="AL89" s="46">
         <v>351</v>
       </c>
-      <c r="AM89" s="45">
+      <c r="AM89" s="27">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="AN89" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN89" s="49">
+      <c r="AO89" s="49">
         <v>3.4849999999999999</v>
       </c>
-      <c r="AO89" s="45">
+      <c r="AP89" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP89" s="49">
+      <c r="AQ89" s="49">
         <v>3.5510000000000002</v>
       </c>
-      <c r="AQ89" t="s">
+      <c r="AR89" t="s">
         <v>259</v>
       </c>
-      <c r="AR89" s="46">
+      <c r="AS89" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="90" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A90" s="40">
         <v>89</v>
       </c>
@@ -13806,26 +14083,29 @@
       <c r="AL90" s="46">
         <v>1436.21</v>
       </c>
-      <c r="AM90" s="45">
+      <c r="AM90" s="27">
+        <v>1.196</v>
+      </c>
+      <c r="AN90" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN90" s="49">
+      <c r="AO90" s="49">
         <v>3.8159999999999998</v>
       </c>
-      <c r="AO90" s="45">
+      <c r="AP90" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP90" s="49">
+      <c r="AQ90" s="49">
         <v>3.6909999999999998</v>
       </c>
-      <c r="AQ90" t="s">
+      <c r="AR90" t="s">
         <v>259</v>
       </c>
-      <c r="AR90" s="46">
+      <c r="AS90" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="91" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A91" s="40">
         <v>90</v>
       </c>
@@ -13940,26 +14220,29 @@
       <c r="AL91" s="46">
         <v>383.52100000000002</v>
       </c>
-      <c r="AM91" s="45">
+      <c r="AM91" s="27">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="AN91" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN91" s="49">
+      <c r="AO91" s="49">
         <v>3.4540000000000002</v>
       </c>
-      <c r="AO91" s="45">
+      <c r="AP91" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP91" s="49">
+      <c r="AQ91" s="49">
         <v>3.835</v>
       </c>
-      <c r="AQ91" t="s">
+      <c r="AR91" t="s">
         <v>259</v>
       </c>
-      <c r="AR91" s="46">
+      <c r="AS91" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="92" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A92" s="40">
         <v>91</v>
       </c>
@@ -14074,26 +14357,29 @@
       <c r="AL92" s="46">
         <v>672.15700000000004</v>
       </c>
-      <c r="AM92" s="45">
+      <c r="AM92" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="AN92" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN92" s="49">
+      <c r="AO92" s="49">
         <v>3.5760000000000001</v>
       </c>
-      <c r="AO92" s="45">
+      <c r="AP92" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP92" s="49">
+      <c r="AQ92" s="49">
         <v>3.7429999999999999</v>
       </c>
-      <c r="AQ92" t="s">
+      <c r="AR92" t="s">
         <v>259</v>
       </c>
-      <c r="AR92" s="46">
+      <c r="AS92" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="93" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A93" s="40">
         <v>92</v>
       </c>
@@ -14208,26 +14494,29 @@
       <c r="AL93" s="46">
         <v>920.99</v>
       </c>
-      <c r="AM93" s="45">
+      <c r="AM93" s="27">
+        <v>0.39100000000000001</v>
+      </c>
+      <c r="AN93" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN93" s="49">
+      <c r="AO93" s="49">
         <v>3.5289999999999999</v>
       </c>
-      <c r="AO93" s="45">
+      <c r="AP93" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP93" s="49">
+      <c r="AQ93" s="49">
         <v>3.8210000000000002</v>
       </c>
-      <c r="AQ93" t="s">
+      <c r="AR93" t="s">
         <v>259</v>
       </c>
-      <c r="AR93" s="46">
+      <c r="AS93" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="94" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A94" s="40">
         <v>93</v>
       </c>
@@ -14342,26 +14631,29 @@
       <c r="AL94" s="46">
         <v>998</v>
       </c>
-      <c r="AM94" s="45">
+      <c r="AM94" s="27">
+        <v>1.113</v>
+      </c>
+      <c r="AN94" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN94" s="49">
+      <c r="AO94" s="49">
         <v>3.7170000000000001</v>
       </c>
-      <c r="AO94" s="45">
+      <c r="AP94" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP94" s="49">
+      <c r="AQ94" s="49">
         <v>3.66</v>
       </c>
-      <c r="AQ94" s="46" t="s">
+      <c r="AR94" s="46" t="s">
         <v>265</v>
       </c>
-      <c r="AR94" s="46">
+      <c r="AS94" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="95" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A95" s="40">
         <v>94</v>
       </c>
@@ -14476,26 +14768,29 @@
       <c r="AL95" s="46">
         <v>1033</v>
       </c>
-      <c r="AM95" s="45">
+      <c r="AM95" s="27">
+        <v>0.61</v>
+      </c>
+      <c r="AN95" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN95" s="49">
+      <c r="AO95" s="49">
         <v>3.62</v>
       </c>
-      <c r="AO95" s="45">
+      <c r="AP95" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP95" s="49">
+      <c r="AQ95" s="49">
         <v>4.0209999999999999</v>
       </c>
-      <c r="AQ95" s="46" t="s">
+      <c r="AR95" s="46" t="s">
         <v>259</v>
       </c>
-      <c r="AR95" s="46">
+      <c r="AS95" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="96" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A96" s="40">
         <v>95</v>
       </c>
@@ -14610,26 +14905,29 @@
       <c r="AL96" s="46">
         <v>1689.8</v>
       </c>
-      <c r="AM96" s="45">
+      <c r="AM96" s="27">
+        <v>1.127</v>
+      </c>
+      <c r="AN96" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN96" s="49">
+      <c r="AO96" s="49">
         <v>3.7839999999999998</v>
       </c>
-      <c r="AO96" s="45">
+      <c r="AP96" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP96" s="49">
+      <c r="AQ96" s="49">
         <v>3.649</v>
       </c>
-      <c r="AQ96" s="46" t="s">
+      <c r="AR96" s="46" t="s">
         <v>262</v>
       </c>
-      <c r="AR96" s="46">
+      <c r="AS96" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="97" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A97" s="40">
         <v>96</v>
       </c>
@@ -14744,26 +15042,29 @@
       <c r="AL97" s="46">
         <v>1513</v>
       </c>
-      <c r="AM97" s="45">
+      <c r="AM97" s="27">
+        <v>0.72799999999999998</v>
+      </c>
+      <c r="AN97" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN97" s="49">
+      <c r="AO97" s="49">
         <v>3.601</v>
       </c>
-      <c r="AO97" s="45">
+      <c r="AP97" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP97" s="49">
+      <c r="AQ97" s="49">
         <v>3.742</v>
       </c>
-      <c r="AQ97" s="46" t="s">
+      <c r="AR97" s="46" t="s">
         <v>259</v>
       </c>
-      <c r="AR97" s="46">
+      <c r="AS97" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="98" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A98" s="40">
         <v>97</v>
       </c>
@@ -14878,26 +15179,29 @@
       <c r="AL98" s="46">
         <v>1037</v>
       </c>
-      <c r="AM98" s="45">
+      <c r="AM98" s="27">
+        <v>0.86099999999999999</v>
+      </c>
+      <c r="AN98" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN98" s="49">
+      <c r="AO98" s="49">
         <v>3.673</v>
       </c>
-      <c r="AO98" s="45">
+      <c r="AP98" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP98" s="49">
+      <c r="AQ98" s="49">
         <v>3.7629999999999999</v>
       </c>
-      <c r="AQ98" s="46" t="s">
+      <c r="AR98" s="46" t="s">
         <v>259</v>
       </c>
-      <c r="AR98" s="46">
+      <c r="AS98" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="99" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A99" s="40">
         <v>98</v>
       </c>
@@ -15012,26 +15316,29 @@
       <c r="AL99" s="46">
         <v>1201</v>
       </c>
-      <c r="AM99" s="45">
+      <c r="AM99" s="27">
+        <v>0.439</v>
+      </c>
+      <c r="AN99" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN99" s="49">
+      <c r="AO99" s="49">
         <v>3.528</v>
       </c>
-      <c r="AO99" s="45">
+      <c r="AP99" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP99" s="49">
+      <c r="AQ99" s="49">
         <v>3.8330000000000002</v>
       </c>
-      <c r="AQ99" s="46" t="s">
+      <c r="AR99" s="46" t="s">
         <v>259</v>
       </c>
-      <c r="AR99" s="46">
+      <c r="AS99" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="100" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A100" s="40">
         <v>99</v>
       </c>
@@ -15146,26 +15453,29 @@
       <c r="AL100" s="46">
         <v>1544</v>
       </c>
-      <c r="AM100" s="45">
+      <c r="AM100" s="27">
+        <v>1.5169999999999999</v>
+      </c>
+      <c r="AN100" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN100" s="49">
+      <c r="AO100" s="49">
         <v>3.823</v>
       </c>
-      <c r="AO100" s="45">
+      <c r="AP100" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP100" s="49">
+      <c r="AQ100" s="49">
         <v>4.0199999999999996</v>
       </c>
-      <c r="AQ100" s="46" t="s">
+      <c r="AR100" s="46" t="s">
         <v>259</v>
       </c>
-      <c r="AR100" s="46">
+      <c r="AS100" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="101" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A101" s="40">
         <v>100</v>
       </c>
@@ -15280,26 +15590,29 @@
       <c r="AL101" s="46">
         <v>683.20899999999995</v>
       </c>
-      <c r="AM101" s="45">
+      <c r="AM101" s="27">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="AN101" s="45">
         <v>3.423</v>
       </c>
-      <c r="AN101" s="49">
+      <c r="AO101" s="49">
         <v>3.605</v>
       </c>
-      <c r="AO101" s="45">
+      <c r="AP101" s="45">
         <v>3.423</v>
       </c>
-      <c r="AP101" s="49">
+      <c r="AQ101" s="49">
         <v>3.883</v>
       </c>
-      <c r="AQ101" s="46" t="s">
+      <c r="AR101" s="46" t="s">
         <v>259</v>
       </c>
-      <c r="AR101" s="46">
+      <c r="AS101" s="46">
         <v>80</v>
       </c>
     </row>
-    <row r="102" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:45" x14ac:dyDescent="0.25">
       <c r="V102" s="2"/>
       <c r="Y102" s="2"/>
       <c r="Z102" s="24"/>
@@ -15309,12 +15622,12 @@
       <c r="AD102" s="25"/>
       <c r="AE102" s="30"/>
       <c r="AF102" s="30"/>
-      <c r="AM102" s="2"/>
       <c r="AN102" s="2"/>
       <c r="AO102" s="2"/>
       <c r="AP102" s="2"/>
-    </row>
-    <row r="103" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AQ102" s="2"/>
+    </row>
+    <row r="103" spans="1:45" x14ac:dyDescent="0.25">
       <c r="V103" s="2"/>
       <c r="Y103" s="2"/>
       <c r="Z103" s="24"/>
@@ -15328,14 +15641,14 @@
       <c r="AJ103" s="24"/>
       <c r="AK103" s="24"/>
       <c r="AL103" s="48"/>
-      <c r="AM103" s="2"/>
       <c r="AN103" s="2"/>
       <c r="AO103" s="2"/>
       <c r="AP103" s="2"/>
       <c r="AQ103" s="2"/>
       <c r="AR103" s="2"/>
-    </row>
-    <row r="104" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AS103" s="2"/>
+    </row>
+    <row r="104" spans="1:45" x14ac:dyDescent="0.25">
       <c r="V104" s="2"/>
       <c r="Y104" s="2"/>
       <c r="Z104" s="2"/>
@@ -15345,14 +15658,14 @@
       <c r="AJ104" s="2"/>
       <c r="AK104" s="2"/>
       <c r="AL104" s="48"/>
-      <c r="AM104" s="2"/>
       <c r="AN104" s="2"/>
       <c r="AO104" s="2"/>
       <c r="AP104" s="2"/>
       <c r="AQ104" s="2"/>
       <c r="AR104" s="2"/>
-    </row>
-    <row r="105" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AS104" s="2"/>
+    </row>
+    <row r="105" spans="1:45" x14ac:dyDescent="0.25">
       <c r="V105" s="2"/>
       <c r="Y105" s="2"/>
       <c r="Z105" s="2"/>
@@ -15362,14 +15675,14 @@
       <c r="AJ105" s="2"/>
       <c r="AK105" s="2"/>
       <c r="AL105" s="48"/>
-      <c r="AM105" s="2"/>
       <c r="AN105" s="2"/>
       <c r="AO105" s="2"/>
       <c r="AP105" s="2"/>
       <c r="AQ105" s="2"/>
       <c r="AR105" s="2"/>
-    </row>
-    <row r="106" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AS105" s="2"/>
+    </row>
+    <row r="106" spans="1:45" x14ac:dyDescent="0.25">
       <c r="V106" s="2"/>
       <c r="Y106" s="2"/>
       <c r="Z106" s="2"/>
@@ -15379,14 +15692,14 @@
       <c r="AJ106" s="2"/>
       <c r="AK106" s="2"/>
       <c r="AL106" s="48"/>
-      <c r="AM106" s="2"/>
       <c r="AN106" s="2"/>
       <c r="AO106" s="2"/>
       <c r="AP106" s="2"/>
       <c r="AQ106" s="2"/>
       <c r="AR106" s="2"/>
-    </row>
-    <row r="107" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AS106" s="2"/>
+    </row>
+    <row r="107" spans="1:45" x14ac:dyDescent="0.25">
       <c r="V107" s="2"/>
       <c r="Y107" s="2"/>
       <c r="Z107" s="2"/>
@@ -15396,14 +15709,14 @@
       <c r="AJ107" s="2"/>
       <c r="AK107" s="2"/>
       <c r="AL107" s="48"/>
-      <c r="AM107" s="2"/>
       <c r="AN107" s="2"/>
       <c r="AO107" s="2"/>
       <c r="AP107" s="2"/>
       <c r="AQ107" s="2"/>
       <c r="AR107" s="2"/>
-    </row>
-    <row r="108" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AS107" s="2"/>
+    </row>
+    <row r="108" spans="1:45" x14ac:dyDescent="0.25">
       <c r="V108" s="2"/>
       <c r="Y108" s="2"/>
       <c r="Z108" s="2"/>
@@ -15413,14 +15726,14 @@
       <c r="AJ108" s="2"/>
       <c r="AK108" s="2"/>
       <c r="AL108" s="48"/>
-      <c r="AM108" s="2"/>
       <c r="AN108" s="2"/>
       <c r="AO108" s="2"/>
       <c r="AP108" s="2"/>
       <c r="AQ108" s="2"/>
       <c r="AR108" s="2"/>
-    </row>
-    <row r="109" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AS108" s="2"/>
+    </row>
+    <row r="109" spans="1:45" x14ac:dyDescent="0.25">
       <c r="V109" s="2"/>
       <c r="Y109" s="2"/>
       <c r="Z109" s="2"/>
@@ -15430,14 +15743,14 @@
       <c r="AJ109" s="2"/>
       <c r="AK109" s="2"/>
       <c r="AL109" s="48"/>
-      <c r="AM109" s="2"/>
       <c r="AN109" s="2"/>
       <c r="AO109" s="2"/>
       <c r="AP109" s="2"/>
       <c r="AQ109" s="2"/>
       <c r="AR109" s="2"/>
-    </row>
-    <row r="110" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AS109" s="2"/>
+    </row>
+    <row r="110" spans="1:45" x14ac:dyDescent="0.25">
       <c r="V110" s="2"/>
       <c r="Y110" s="2"/>
       <c r="Z110" s="2"/>
@@ -15447,14 +15760,14 @@
       <c r="AJ110" s="2"/>
       <c r="AK110" s="2"/>
       <c r="AL110" s="48"/>
-      <c r="AM110" s="2"/>
       <c r="AN110" s="2"/>
       <c r="AO110" s="2"/>
       <c r="AP110" s="2"/>
       <c r="AQ110" s="2"/>
       <c r="AR110" s="2"/>
-    </row>
-    <row r="111" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AS110" s="2"/>
+    </row>
+    <row r="111" spans="1:45" x14ac:dyDescent="0.25">
       <c r="V111" s="2"/>
       <c r="Y111" s="2"/>
       <c r="Z111" s="2"/>
@@ -15464,14 +15777,14 @@
       <c r="AJ111" s="2"/>
       <c r="AK111" s="2"/>
       <c r="AL111" s="48"/>
-      <c r="AM111" s="2"/>
       <c r="AN111" s="2"/>
       <c r="AO111" s="2"/>
       <c r="AP111" s="2"/>
       <c r="AQ111" s="2"/>
       <c r="AR111" s="2"/>
-    </row>
-    <row r="112" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AS111" s="2"/>
+    </row>
+    <row r="112" spans="1:45" x14ac:dyDescent="0.25">
       <c r="V112" s="2"/>
       <c r="Y112" s="2"/>
       <c r="Z112" s="2"/>
@@ -15481,26 +15794,26 @@
       <c r="AJ112" s="2"/>
       <c r="AK112" s="2"/>
       <c r="AL112" s="48"/>
-      <c r="AM112" s="2"/>
       <c r="AN112" s="2"/>
       <c r="AO112" s="2"/>
       <c r="AP112" s="2"/>
       <c r="AQ112" s="2"/>
       <c r="AR112" s="2"/>
-    </row>
-    <row r="113" spans="22:44" x14ac:dyDescent="0.25">
+      <c r="AS112" s="2"/>
+    </row>
+    <row r="113" spans="22:45" x14ac:dyDescent="0.25">
       <c r="V113" s="2"/>
       <c r="Y113" s="2"/>
       <c r="Z113" s="2"/>
       <c r="AA113" s="2"/>
       <c r="AB113" s="2"/>
       <c r="AC113" s="2"/>
-      <c r="AM113" s="2"/>
       <c r="AN113" s="2"/>
       <c r="AO113" s="2"/>
       <c r="AP113" s="2"/>
-    </row>
-    <row r="114" spans="22:44" x14ac:dyDescent="0.25">
+      <c r="AQ113" s="2"/>
+    </row>
+    <row r="114" spans="22:45" x14ac:dyDescent="0.25">
       <c r="V114" s="2"/>
       <c r="Y114" s="2"/>
       <c r="Z114" s="2"/>
@@ -15511,12 +15824,12 @@
       <c r="AH114" s="19"/>
       <c r="AJ114" s="33"/>
       <c r="AK114" s="33"/>
-      <c r="AM114" s="2"/>
       <c r="AN114" s="2"/>
       <c r="AO114" s="2"/>
       <c r="AP114" s="2"/>
-    </row>
-    <row r="115" spans="22:44" x14ac:dyDescent="0.25">
+      <c r="AQ114" s="2"/>
+    </row>
+    <row r="115" spans="22:45" x14ac:dyDescent="0.25">
       <c r="V115" s="2"/>
       <c r="Y115" s="2"/>
       <c r="Z115" s="2"/>
@@ -15526,14 +15839,14 @@
       <c r="AJ115" s="2"/>
       <c r="AK115" s="2"/>
       <c r="AL115" s="48"/>
-      <c r="AM115" s="2"/>
       <c r="AN115" s="2"/>
       <c r="AO115" s="2"/>
       <c r="AP115" s="2"/>
       <c r="AQ115" s="2"/>
       <c r="AR115" s="2"/>
-    </row>
-    <row r="116" spans="22:44" x14ac:dyDescent="0.25">
+      <c r="AS115" s="2"/>
+    </row>
+    <row r="116" spans="22:45" x14ac:dyDescent="0.25">
       <c r="V116" s="2"/>
       <c r="Y116" s="2"/>
       <c r="Z116" s="2"/>
@@ -15543,14 +15856,14 @@
       <c r="AJ116" s="2"/>
       <c r="AK116" s="2"/>
       <c r="AL116" s="48"/>
-      <c r="AM116" s="2"/>
       <c r="AN116" s="2"/>
       <c r="AO116" s="2"/>
       <c r="AP116" s="2"/>
       <c r="AQ116" s="2"/>
       <c r="AR116" s="2"/>
-    </row>
-    <row r="117" spans="22:44" x14ac:dyDescent="0.25">
+      <c r="AS116" s="2"/>
+    </row>
+    <row r="117" spans="22:45" x14ac:dyDescent="0.25">
       <c r="V117" s="2"/>
       <c r="Y117" s="2"/>
       <c r="Z117" s="2"/>
@@ -15560,14 +15873,14 @@
       <c r="AJ117" s="2"/>
       <c r="AK117" s="2"/>
       <c r="AL117" s="48"/>
-      <c r="AM117" s="2"/>
       <c r="AN117" s="2"/>
       <c r="AO117" s="2"/>
       <c r="AP117" s="2"/>
       <c r="AQ117" s="2"/>
       <c r="AR117" s="2"/>
-    </row>
-    <row r="118" spans="22:44" x14ac:dyDescent="0.25">
+      <c r="AS117" s="2"/>
+    </row>
+    <row r="118" spans="22:45" x14ac:dyDescent="0.25">
       <c r="V118" s="2"/>
       <c r="Y118" s="2"/>
       <c r="Z118" s="2"/>
@@ -15577,14 +15890,14 @@
       <c r="AJ118" s="2"/>
       <c r="AK118" s="2"/>
       <c r="AL118" s="48"/>
-      <c r="AM118" s="2"/>
       <c r="AN118" s="2"/>
       <c r="AO118" s="2"/>
       <c r="AP118" s="2"/>
       <c r="AQ118" s="2"/>
       <c r="AR118" s="2"/>
-    </row>
-    <row r="119" spans="22:44" x14ac:dyDescent="0.25">
+      <c r="AS118" s="2"/>
+    </row>
+    <row r="119" spans="22:45" x14ac:dyDescent="0.25">
       <c r="V119" s="2"/>
       <c r="Y119" s="2"/>
       <c r="Z119" s="2"/>
@@ -15594,14 +15907,14 @@
       <c r="AJ119" s="2"/>
       <c r="AK119" s="2"/>
       <c r="AL119" s="48"/>
-      <c r="AM119" s="2"/>
       <c r="AN119" s="2"/>
       <c r="AO119" s="2"/>
       <c r="AP119" s="2"/>
       <c r="AQ119" s="2"/>
       <c r="AR119" s="2"/>
-    </row>
-    <row r="120" spans="22:44" x14ac:dyDescent="0.25">
+      <c r="AS119" s="2"/>
+    </row>
+    <row r="120" spans="22:45" x14ac:dyDescent="0.25">
       <c r="V120" s="2"/>
       <c r="Y120" s="2"/>
       <c r="Z120" s="2"/>
@@ -15611,14 +15924,14 @@
       <c r="AJ120" s="2"/>
       <c r="AK120" s="2"/>
       <c r="AL120" s="48"/>
-      <c r="AM120" s="2"/>
       <c r="AN120" s="2"/>
       <c r="AO120" s="2"/>
       <c r="AP120" s="2"/>
       <c r="AQ120" s="2"/>
       <c r="AR120" s="2"/>
-    </row>
-    <row r="121" spans="22:44" x14ac:dyDescent="0.25">
+      <c r="AS120" s="2"/>
+    </row>
+    <row r="121" spans="22:45" x14ac:dyDescent="0.25">
       <c r="V121" s="2"/>
       <c r="Y121" s="2"/>
       <c r="Z121" s="2"/>
@@ -15629,18 +15942,18 @@
       <c r="AH121" s="19"/>
       <c r="AJ121" s="33"/>
       <c r="AK121" s="33"/>
-      <c r="AM121" s="2"/>
       <c r="AN121" s="2"/>
       <c r="AO121" s="2"/>
       <c r="AP121" s="2"/>
-    </row>
-    <row r="126" spans="22:44" x14ac:dyDescent="0.25">
+      <c r="AQ121" s="2"/>
+    </row>
+    <row r="126" spans="22:45" x14ac:dyDescent="0.25">
       <c r="AG126" s="30"/>
       <c r="AJ126" s="24"/>
       <c r="AK126" s="24"/>
       <c r="AL126" s="48"/>
-      <c r="AQ126" s="2"/>
       <c r="AR126" s="2"/>
+      <c r="AS126" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -15651,10 +15964,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:X122"/>
+  <dimension ref="A1:X123"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16454,79 +16767,83 @@
       <c r="W39" s="8"/>
       <c r="X39" s="8"/>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:24" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="28" t="s">
+        <v>268</v>
+      </c>
+      <c r="B40" s="26" t="s">
+        <v>270</v>
+      </c>
+      <c r="C40" s="26" t="s">
+        <v>231</v>
+      </c>
+      <c r="D40" s="26" t="s">
+        <v>269</v>
+      </c>
+      <c r="G40" s="28"/>
+      <c r="K40" s="27"/>
+      <c r="L40" s="27"/>
+      <c r="M40" s="27"/>
+      <c r="Q40" s="25"/>
+      <c r="R40" s="25"/>
+      <c r="S40" s="25"/>
+      <c r="T40" s="25"/>
+      <c r="U40" s="25"/>
+      <c r="V40" s="25"/>
+      <c r="W40" s="25"/>
+      <c r="X40" s="25"/>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A41" s="28" t="s">
         <v>247</v>
       </c>
-      <c r="B40" s="26" t="s">
+      <c r="B41" s="26" t="s">
         <v>251</v>
-      </c>
-      <c r="D40" s="26" t="s">
-        <v>200</v>
-      </c>
-      <c r="K40" s="12"/>
-      <c r="L40" s="12"/>
-      <c r="M40" s="12"/>
-      <c r="Q40" s="8"/>
-      <c r="R40" s="8"/>
-      <c r="S40" s="8"/>
-      <c r="T40" s="8"/>
-      <c r="U40" s="8"/>
-      <c r="V40" s="8"/>
-      <c r="W40" s="8"/>
-      <c r="X40" s="8"/>
-    </row>
-    <row r="41" spans="1:24" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="28" t="s">
-        <v>248</v>
-      </c>
-      <c r="B41" s="26" t="s">
-        <v>254</v>
       </c>
       <c r="D41" s="26" t="s">
         <v>200</v>
       </c>
-      <c r="G41" s="28"/>
-      <c r="K41" s="27"/>
-      <c r="L41" s="27"/>
-      <c r="M41" s="27"/>
-      <c r="Q41" s="25"/>
-      <c r="R41" s="25"/>
-      <c r="S41" s="25"/>
-      <c r="T41" s="25"/>
-      <c r="U41" s="25"/>
-      <c r="V41" s="25"/>
-      <c r="W41" s="25"/>
-      <c r="X41" s="25"/>
-    </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="K41" s="12"/>
+      <c r="L41" s="12"/>
+      <c r="M41" s="12"/>
+      <c r="Q41" s="8"/>
+      <c r="R41" s="8"/>
+      <c r="S41" s="8"/>
+      <c r="T41" s="8"/>
+      <c r="U41" s="8"/>
+      <c r="V41" s="8"/>
+      <c r="W41" s="8"/>
+      <c r="X41" s="8"/>
+    </row>
+    <row r="42" spans="1:24" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="28" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B42" s="26" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D42" s="26" t="s">
         <v>200</v>
       </c>
-      <c r="K42" s="12"/>
-      <c r="L42" s="12"/>
-      <c r="M42" s="12"/>
-      <c r="Q42" s="8"/>
-      <c r="R42" s="8"/>
-      <c r="S42" s="8"/>
-      <c r="T42" s="8"/>
-      <c r="U42" s="8"/>
-      <c r="V42" s="8"/>
-      <c r="W42" s="8"/>
-      <c r="X42" s="8"/>
+      <c r="G42" s="28"/>
+      <c r="K42" s="27"/>
+      <c r="L42" s="27"/>
+      <c r="M42" s="27"/>
+      <c r="Q42" s="25"/>
+      <c r="R42" s="25"/>
+      <c r="S42" s="25"/>
+      <c r="T42" s="25"/>
+      <c r="U42" s="25"/>
+      <c r="V42" s="25"/>
+      <c r="W42" s="25"/>
+      <c r="X42" s="25"/>
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43" s="28" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D43" s="26" t="s">
         <v>200</v>
@@ -16535,66 +16852,76 @@
       <c r="L43" s="12"/>
       <c r="M43" s="12"/>
       <c r="Q43" s="8"/>
+      <c r="R43" s="8"/>
       <c r="S43" s="8"/>
       <c r="T43" s="8"/>
       <c r="U43" s="8"/>
+      <c r="V43" s="8"/>
       <c r="W43" s="8"/>
       <c r="X43" s="8"/>
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A44" s="28" t="s">
-        <v>261</v>
-      </c>
-      <c r="B44" s="14"/>
+        <v>250</v>
+      </c>
+      <c r="B44" s="26" t="s">
+        <v>252</v>
+      </c>
+      <c r="D44" s="26" t="s">
+        <v>200</v>
+      </c>
       <c r="K44" s="12"/>
       <c r="L44" s="12"/>
       <c r="M44" s="12"/>
       <c r="Q44" s="8"/>
+      <c r="S44" s="8"/>
+      <c r="T44" s="8"/>
       <c r="U44" s="8"/>
       <c r="W44" s="8"/>
       <c r="X44" s="8"/>
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A45" s="28" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B45" s="14"/>
       <c r="K45" s="12"/>
       <c r="L45" s="12"/>
       <c r="M45" s="12"/>
       <c r="Q45" s="8"/>
-      <c r="T45" s="8"/>
       <c r="U45" s="8"/>
+      <c r="W45" s="8"/>
       <c r="X45" s="8"/>
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A46" s="19"/>
+      <c r="A46" s="28" t="s">
+        <v>260</v>
+      </c>
+      <c r="B46" s="14"/>
       <c r="K46" s="12"/>
       <c r="L46" s="12"/>
       <c r="M46" s="12"/>
       <c r="Q46" s="8"/>
+      <c r="T46" s="8"/>
       <c r="U46" s="8"/>
+      <c r="X46" s="8"/>
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A47" s="19"/>
       <c r="K47" s="12"/>
       <c r="L47" s="12"/>
       <c r="M47" s="12"/>
       <c r="Q47" s="8"/>
-      <c r="R47" s="8"/>
-      <c r="S47" s="8"/>
-      <c r="T47" s="8"/>
       <c r="U47" s="8"/>
-      <c r="V47" s="8"/>
-      <c r="W47" s="8"/>
-      <c r="X47" s="8"/>
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A48" s="19"/>
       <c r="K48" s="12"/>
       <c r="L48" s="12"/>
       <c r="M48" s="12"/>
       <c r="Q48" s="8"/>
       <c r="R48" s="8"/>
+      <c r="S48" s="8"/>
+      <c r="T48" s="8"/>
       <c r="U48" s="8"/>
       <c r="V48" s="8"/>
       <c r="W48" s="8"/>
@@ -16619,8 +16946,6 @@
       <c r="M50" s="12"/>
       <c r="Q50" s="8"/>
       <c r="R50" s="8"/>
-      <c r="S50" s="8"/>
-      <c r="T50" s="8"/>
       <c r="U50" s="8"/>
       <c r="V50" s="8"/>
       <c r="W50" s="8"/>
@@ -16647,6 +16972,8 @@
       <c r="M52" s="12"/>
       <c r="Q52" s="8"/>
       <c r="R52" s="8"/>
+      <c r="S52" s="8"/>
+      <c r="T52" s="8"/>
       <c r="U52" s="8"/>
       <c r="V52" s="8"/>
       <c r="W52" s="8"/>
@@ -16659,8 +16986,6 @@
       <c r="M53" s="12"/>
       <c r="Q53" s="8"/>
       <c r="R53" s="8"/>
-      <c r="S53" s="8"/>
-      <c r="T53" s="8"/>
       <c r="U53" s="8"/>
       <c r="V53" s="8"/>
       <c r="W53" s="8"/>
@@ -16701,6 +17026,8 @@
       <c r="M56" s="12"/>
       <c r="Q56" s="8"/>
       <c r="R56" s="8"/>
+      <c r="S56" s="8"/>
+      <c r="T56" s="8"/>
       <c r="U56" s="8"/>
       <c r="V56" s="8"/>
       <c r="W56" s="8"/>
@@ -16713,8 +17040,6 @@
       <c r="M57" s="12"/>
       <c r="Q57" s="8"/>
       <c r="R57" s="8"/>
-      <c r="S57" s="8"/>
-      <c r="T57" s="8"/>
       <c r="U57" s="8"/>
       <c r="V57" s="8"/>
       <c r="W57" s="8"/>
@@ -16796,9 +17121,11 @@
       <c r="L63" s="12"/>
       <c r="M63" s="12"/>
       <c r="Q63" s="8"/>
+      <c r="R63" s="8"/>
       <c r="S63" s="8"/>
       <c r="T63" s="8"/>
       <c r="U63" s="8"/>
+      <c r="V63" s="8"/>
       <c r="W63" s="8"/>
       <c r="X63" s="8"/>
     </row>
@@ -16808,7 +17135,6 @@
       <c r="L64" s="12"/>
       <c r="M64" s="12"/>
       <c r="Q64" s="8"/>
-      <c r="R64" s="8"/>
       <c r="S64" s="8"/>
       <c r="T64" s="8"/>
       <c r="U64" s="8"/>
@@ -16825,7 +17151,6 @@
       <c r="S65" s="8"/>
       <c r="T65" s="8"/>
       <c r="U65" s="8"/>
-      <c r="V65" s="8"/>
       <c r="W65" s="8"/>
       <c r="X65" s="8"/>
     </row>
@@ -16839,6 +17164,7 @@
       <c r="S66" s="8"/>
       <c r="T66" s="8"/>
       <c r="U66" s="8"/>
+      <c r="V66" s="8"/>
       <c r="W66" s="8"/>
       <c r="X66" s="8"/>
     </row>
@@ -16852,7 +17178,6 @@
       <c r="S67" s="8"/>
       <c r="T67" s="8"/>
       <c r="U67" s="8"/>
-      <c r="V67" s="8"/>
       <c r="W67" s="8"/>
       <c r="X67" s="8"/>
     </row>
@@ -17068,13 +17393,13 @@
     </row>
     <row r="83" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A83" s="19"/>
-      <c r="H83" s="19"/>
-      <c r="I83" s="19"/>
       <c r="K83" s="12"/>
       <c r="L83" s="12"/>
       <c r="M83" s="12"/>
       <c r="Q83" s="8"/>
       <c r="R83" s="8"/>
+      <c r="S83" s="8"/>
+      <c r="T83" s="8"/>
       <c r="U83" s="8"/>
       <c r="V83" s="8"/>
       <c r="W83" s="8"/>
@@ -17089,8 +17414,6 @@
       <c r="M84" s="12"/>
       <c r="Q84" s="8"/>
       <c r="R84" s="8"/>
-      <c r="S84" s="8"/>
-      <c r="T84" s="8"/>
       <c r="U84" s="8"/>
       <c r="V84" s="8"/>
       <c r="W84" s="8"/>
@@ -17124,6 +17447,8 @@
       <c r="S86" s="8"/>
       <c r="T86" s="8"/>
       <c r="U86" s="8"/>
+      <c r="V86" s="8"/>
+      <c r="W86" s="8"/>
       <c r="X86" s="8"/>
     </row>
     <row r="87" spans="1:24" x14ac:dyDescent="0.25">
@@ -17138,8 +17463,6 @@
       <c r="S87" s="8"/>
       <c r="T87" s="8"/>
       <c r="U87" s="8"/>
-      <c r="V87" s="8"/>
-      <c r="W87" s="8"/>
       <c r="X87" s="8"/>
     </row>
     <row r="88" spans="1:24" x14ac:dyDescent="0.25">
@@ -17358,9 +17681,11 @@
       <c r="L101" s="12"/>
       <c r="M101" s="12"/>
       <c r="Q101" s="8"/>
+      <c r="R101" s="8"/>
       <c r="S101" s="8"/>
       <c r="T101" s="8"/>
       <c r="U101" s="8"/>
+      <c r="V101" s="8"/>
       <c r="W101" s="8"/>
       <c r="X101" s="8"/>
     </row>
@@ -17372,32 +17697,27 @@
       <c r="L102" s="12"/>
       <c r="M102" s="12"/>
       <c r="Q102" s="8"/>
+      <c r="S102" s="8"/>
+      <c r="T102" s="8"/>
       <c r="U102" s="8"/>
+      <c r="W102" s="8"/>
+      <c r="X102" s="8"/>
     </row>
     <row r="103" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A103" s="19"/>
       <c r="H103" s="19"/>
       <c r="I103" s="19"/>
-      <c r="J103" s="19"/>
       <c r="K103" s="12"/>
       <c r="L103" s="12"/>
       <c r="M103" s="12"/>
-      <c r="N103" s="12"/>
-      <c r="O103" s="12"/>
-      <c r="P103" s="12"/>
       <c r="Q103" s="8"/>
-      <c r="R103" s="8"/>
-      <c r="S103" s="8"/>
-      <c r="T103" s="8"/>
       <c r="U103" s="8"/>
-      <c r="V103" s="8"/>
-      <c r="W103" s="8"/>
-      <c r="X103" s="8"/>
     </row>
     <row r="104" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A104" s="19"/>
       <c r="H104" s="19"/>
       <c r="I104" s="19"/>
+      <c r="J104" s="19"/>
       <c r="K104" s="12"/>
       <c r="L104" s="12"/>
       <c r="M104" s="12"/>
@@ -17417,7 +17737,6 @@
       <c r="A105" s="19"/>
       <c r="H105" s="19"/>
       <c r="I105" s="19"/>
-      <c r="J105" s="19"/>
       <c r="K105" s="12"/>
       <c r="L105" s="12"/>
       <c r="M105" s="12"/>
@@ -17437,6 +17756,7 @@
       <c r="A106" s="19"/>
       <c r="H106" s="19"/>
       <c r="I106" s="19"/>
+      <c r="J106" s="19"/>
       <c r="K106" s="12"/>
       <c r="L106" s="12"/>
       <c r="M106" s="12"/>
@@ -17456,7 +17776,6 @@
       <c r="A107" s="19"/>
       <c r="H107" s="19"/>
       <c r="I107" s="19"/>
-      <c r="J107" s="19"/>
       <c r="K107" s="12"/>
       <c r="L107" s="12"/>
       <c r="M107" s="12"/>
@@ -17476,6 +17795,7 @@
       <c r="A108" s="19"/>
       <c r="H108" s="19"/>
       <c r="I108" s="19"/>
+      <c r="J108" s="19"/>
       <c r="K108" s="12"/>
       <c r="L108" s="12"/>
       <c r="M108" s="12"/>
@@ -17495,7 +17815,6 @@
       <c r="A109" s="19"/>
       <c r="H109" s="19"/>
       <c r="I109" s="19"/>
-      <c r="J109" s="19"/>
       <c r="K109" s="12"/>
       <c r="L109" s="12"/>
       <c r="M109" s="12"/>
@@ -17515,6 +17834,7 @@
       <c r="A110" s="19"/>
       <c r="H110" s="19"/>
       <c r="I110" s="19"/>
+      <c r="J110" s="19"/>
       <c r="K110" s="12"/>
       <c r="L110" s="12"/>
       <c r="M110" s="12"/>
@@ -17534,7 +17854,6 @@
       <c r="A111" s="19"/>
       <c r="H111" s="19"/>
       <c r="I111" s="19"/>
-      <c r="J111" s="19"/>
       <c r="K111" s="12"/>
       <c r="L111" s="12"/>
       <c r="M111" s="12"/>
@@ -17554,6 +17873,7 @@
       <c r="A112" s="19"/>
       <c r="H112" s="19"/>
       <c r="I112" s="19"/>
+      <c r="J112" s="19"/>
       <c r="K112" s="12"/>
       <c r="L112" s="12"/>
       <c r="M112" s="12"/>
@@ -17573,7 +17893,6 @@
       <c r="A113" s="19"/>
       <c r="H113" s="19"/>
       <c r="I113" s="19"/>
-      <c r="J113" s="19"/>
       <c r="K113" s="12"/>
       <c r="L113" s="12"/>
       <c r="M113" s="12"/>
@@ -17593,6 +17912,7 @@
       <c r="A114" s="19"/>
       <c r="H114" s="19"/>
       <c r="I114" s="19"/>
+      <c r="J114" s="19"/>
       <c r="K114" s="12"/>
       <c r="L114" s="12"/>
       <c r="M114" s="12"/>
@@ -17612,7 +17932,6 @@
       <c r="A115" s="19"/>
       <c r="H115" s="19"/>
       <c r="I115" s="19"/>
-      <c r="J115" s="19"/>
       <c r="K115" s="12"/>
       <c r="L115" s="12"/>
       <c r="M115" s="12"/>
@@ -17632,6 +17951,7 @@
       <c r="A116" s="19"/>
       <c r="H116" s="19"/>
       <c r="I116" s="19"/>
+      <c r="J116" s="19"/>
       <c r="K116" s="12"/>
       <c r="L116" s="12"/>
       <c r="M116" s="12"/>
@@ -17651,7 +17971,6 @@
       <c r="A117" s="19"/>
       <c r="H117" s="19"/>
       <c r="I117" s="19"/>
-      <c r="J117" s="19"/>
       <c r="K117" s="12"/>
       <c r="L117" s="12"/>
       <c r="M117" s="12"/>
@@ -17671,6 +17990,7 @@
       <c r="A118" s="19"/>
       <c r="H118" s="19"/>
       <c r="I118" s="19"/>
+      <c r="J118" s="19"/>
       <c r="K118" s="12"/>
       <c r="L118" s="12"/>
       <c r="M118" s="12"/>
@@ -17690,7 +18010,6 @@
       <c r="A119" s="19"/>
       <c r="H119" s="19"/>
       <c r="I119" s="19"/>
-      <c r="J119" s="19"/>
       <c r="K119" s="12"/>
       <c r="L119" s="12"/>
       <c r="M119" s="12"/>
@@ -17710,6 +18029,7 @@
       <c r="A120" s="19"/>
       <c r="H120" s="19"/>
       <c r="I120" s="19"/>
+      <c r="J120" s="19"/>
       <c r="K120" s="12"/>
       <c r="L120" s="12"/>
       <c r="M120" s="12"/>
@@ -17729,7 +18049,6 @@
       <c r="A121" s="19"/>
       <c r="H121" s="19"/>
       <c r="I121" s="19"/>
-      <c r="J121" s="19"/>
       <c r="K121" s="12"/>
       <c r="L121" s="12"/>
       <c r="M121" s="12"/>
@@ -17749,6 +18068,7 @@
       <c r="A122" s="19"/>
       <c r="H122" s="19"/>
       <c r="I122" s="19"/>
+      <c r="J122" s="19"/>
       <c r="K122" s="12"/>
       <c r="L122" s="12"/>
       <c r="M122" s="12"/>
@@ -17763,6 +18083,25 @@
       <c r="V122" s="8"/>
       <c r="W122" s="8"/>
       <c r="X122" s="8"/>
+    </row>
+    <row r="123" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A123" s="19"/>
+      <c r="H123" s="19"/>
+      <c r="I123" s="19"/>
+      <c r="K123" s="12"/>
+      <c r="L123" s="12"/>
+      <c r="M123" s="12"/>
+      <c r="N123" s="12"/>
+      <c r="O123" s="12"/>
+      <c r="P123" s="12"/>
+      <c r="Q123" s="8"/>
+      <c r="R123" s="8"/>
+      <c r="S123" s="8"/>
+      <c r="T123" s="8"/>
+      <c r="U123" s="8"/>
+      <c r="V123" s="8"/>
+      <c r="W123" s="8"/>
+      <c r="X123" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>